<commit_message>
Fix manual mode for money leaderboard
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1936,7 +1936,7 @@
       <c r="A14" s="101" t="n"/>
       <c r="B14" s="124" t="inlineStr">
         <is>
-          <t>Dernière update le 05.03.25 à 01:37</t>
+          <t>Dernière update le 05.03.25 à 01:59</t>
         </is>
       </c>
       <c r="Q14" s="101" t="n"/>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="I8" s="135" t="inlineStr">
         <is>
-          <t>Terraciid</t>
+          <t>LuttiLutti</t>
         </is>
       </c>
       <c r="J8" s="137" t="n">
@@ -2432,7 +2432,7 @@
       </c>
       <c r="L8" s="135" t="inlineStr">
         <is>
-          <t>Maxouzboub</t>
+          <t>nemenems</t>
         </is>
       </c>
       <c r="M8" s="139" t="n">
@@ -2488,7 +2488,7 @@
       </c>
       <c r="I9" s="128" t="inlineStr">
         <is>
-          <t>LuttiLutti</t>
+          <t>KyriaaTV</t>
         </is>
       </c>
       <c r="J9" s="141" t="n">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="L9" s="128" t="inlineStr">
         <is>
-          <t>nemenems</t>
+          <t>Maxouzboub</t>
         </is>
       </c>
       <c r="M9" s="143" t="n">
@@ -2548,7 +2548,7 @@
       </c>
       <c r="I10" s="135" t="inlineStr">
         <is>
-          <t>KyriaaTV</t>
+          <t>Terraciid</t>
         </is>
       </c>
       <c r="J10" s="137" t="n">
@@ -2753,7 +2753,7 @@
       <c r="A14" s="126" t="n"/>
       <c r="B14" s="147" t="inlineStr">
         <is>
-          <t>Dernière update le 05.03.25 à 01:37</t>
+          <t>Dernière update le 05.03.25 à 01:59</t>
         </is>
       </c>
       <c r="Q14" s="126" t="n"/>
@@ -2899,7 +2899,7 @@
       </c>
       <c r="I3" s="153" t="inlineStr">
         <is>
-          <t>JLTootmy</t>
+          <t>Kaatsup</t>
         </is>
       </c>
       <c r="J3" s="154" t="n">
@@ -2925,7 +2925,7 @@
       </c>
       <c r="O3" s="151" t="inlineStr">
         <is>
-          <t>BagheraJones</t>
+          <t>Elspawn</t>
         </is>
       </c>
       <c r="P3" s="151" t="n">
@@ -2968,7 +2968,7 @@
       </c>
       <c r="I4" s="158" t="inlineStr">
         <is>
-          <t>Terraciid</t>
+          <t>Brybry_</t>
         </is>
       </c>
       <c r="J4" s="160" t="n">
@@ -3037,7 +3037,7 @@
       </c>
       <c r="I5" s="151" t="inlineStr">
         <is>
-          <t>Brybry_</t>
+          <t>Terraciid</t>
         </is>
       </c>
       <c r="J5" s="167" t="n">
@@ -3063,7 +3063,7 @@
       </c>
       <c r="O5" s="151" t="inlineStr">
         <is>
-          <t>Horty_</t>
+          <t>HarryLafranc</t>
         </is>
       </c>
       <c r="P5" s="151" t="n">
@@ -3119,7 +3119,7 @@
       </c>
       <c r="L6" s="158" t="inlineStr">
         <is>
-          <t>Mynth0s</t>
+          <t>ARELIANN</t>
         </is>
       </c>
       <c r="M6" s="162" t="n">
@@ -3132,7 +3132,7 @@
       </c>
       <c r="O6" s="158" t="inlineStr">
         <is>
-          <t>HarryLafranc</t>
+          <t>Pepito_kawazakii</t>
         </is>
       </c>
       <c r="P6" s="158" t="n">
@@ -3188,7 +3188,7 @@
       </c>
       <c r="L7" s="151" t="inlineStr">
         <is>
-          <t>ARELIANN</t>
+          <t>Mynth0s</t>
         </is>
       </c>
       <c r="M7" s="169" t="n">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="O7" s="151" t="inlineStr">
         <is>
-          <t>Pepito_kawazakii</t>
+          <t>Horty_</t>
         </is>
       </c>
       <c r="P7" s="151" t="n">
@@ -3326,7 +3326,7 @@
       </c>
       <c r="L9" s="151" t="inlineStr">
         <is>
-          <t>Angle_Droit</t>
+          <t>Maxouzboub</t>
         </is>
       </c>
       <c r="M9" s="169" t="n">
@@ -3386,7 +3386,7 @@
       </c>
       <c r="L10" s="158" t="inlineStr">
         <is>
-          <t>Maxouzboub</t>
+          <t>Angle_Droit</t>
         </is>
       </c>
       <c r="M10" s="162" t="n">
@@ -3504,7 +3504,7 @@
       </c>
       <c r="L12" s="158" t="inlineStr">
         <is>
-          <t>Elspawn</t>
+          <t>BagheraJones</t>
         </is>
       </c>
       <c r="M12" s="162" t="n">
@@ -3537,7 +3537,7 @@
       </c>
       <c r="F13" s="151" t="inlineStr">
         <is>
-          <t>Kaatsup</t>
+          <t>JLTootmy</t>
         </is>
       </c>
       <c r="G13" s="151" t="n">
@@ -3578,7 +3578,7 @@
       <c r="A14" s="149" t="n"/>
       <c r="B14" s="173" t="inlineStr">
         <is>
-          <t>Dernière update le 05.03.25 à 01:37</t>
+          <t>Dernière update le 05.03.25 à 01:59</t>
         </is>
       </c>
       <c r="Q14" s="149" t="n"/>
@@ -3711,7 +3711,7 @@
       </c>
       <c r="F3" s="177" t="inlineStr">
         <is>
-          <t>ChloeRamdani</t>
+          <t>AntoineDaniel_</t>
         </is>
       </c>
       <c r="G3" s="177" t="n">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="L3" s="182" t="inlineStr">
         <is>
-          <t>Gom4rt_</t>
+          <t>Terraciid</t>
         </is>
       </c>
       <c r="M3" s="183" t="n">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="O3" s="177" t="inlineStr">
         <is>
-          <t>HarryLafranc</t>
+          <t>Horty_</t>
         </is>
       </c>
       <c r="P3" s="177" t="n">
@@ -3793,7 +3793,7 @@
       </c>
       <c r="I4" s="184" t="inlineStr">
         <is>
-          <t>NakaStream</t>
+          <t>LittleBigWhale</t>
         </is>
       </c>
       <c r="J4" s="186" t="n">
@@ -3806,7 +3806,7 @@
       </c>
       <c r="L4" s="184" t="inlineStr">
         <is>
-          <t>ARELIANN</t>
+          <t>Gom4rt_</t>
         </is>
       </c>
       <c r="M4" s="188" t="n">
@@ -3819,7 +3819,7 @@
       </c>
       <c r="O4" s="184" t="inlineStr">
         <is>
-          <t>nisqylegoat</t>
+          <t>HarryLafranc</t>
         </is>
       </c>
       <c r="P4" s="184" t="n">
@@ -3862,7 +3862,7 @@
       </c>
       <c r="I5" s="177" t="inlineStr">
         <is>
-          <t>LittleBigWhale</t>
+          <t>NakaStream</t>
         </is>
       </c>
       <c r="J5" s="190" t="n">
@@ -3875,7 +3875,7 @@
       </c>
       <c r="L5" s="177" t="inlineStr">
         <is>
-          <t>Maxouzboub</t>
+          <t>Wingobear</t>
         </is>
       </c>
       <c r="M5" s="192" t="n">
@@ -3888,7 +3888,7 @@
       </c>
       <c r="O5" s="177" t="inlineStr">
         <is>
-          <t>Grimkujow</t>
+          <t>Hiro_Ammar</t>
         </is>
       </c>
       <c r="P5" s="177" t="n">
@@ -3944,7 +3944,7 @@
       </c>
       <c r="L6" s="184" t="inlineStr">
         <is>
-          <t>XoTrixy</t>
+          <t>ZeratoR</t>
         </is>
       </c>
       <c r="M6" s="188" t="n">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="O6" s="184" t="inlineStr">
         <is>
-          <t>BagheraJones</t>
+          <t>CrocodyleTV</t>
         </is>
       </c>
       <c r="P6" s="184" t="n">
@@ -4000,7 +4000,7 @@
       </c>
       <c r="I7" s="177" t="inlineStr">
         <is>
-          <t>Angle_Droit</t>
+          <t>Bytell2</t>
         </is>
       </c>
       <c r="J7" s="190" t="n">
@@ -4026,7 +4026,7 @@
       </c>
       <c r="O7" s="177" t="inlineStr">
         <is>
-          <t>Horty_</t>
+          <t>BagheraJones</t>
         </is>
       </c>
       <c r="P7" s="177" t="n">
@@ -4056,7 +4056,7 @@
       </c>
       <c r="F8" s="184" t="inlineStr">
         <is>
-          <t>Etoiles</t>
+          <t>_Linca</t>
         </is>
       </c>
       <c r="G8" s="184" t="n">
@@ -4069,7 +4069,7 @@
       </c>
       <c r="I8" s="184" t="inlineStr">
         <is>
-          <t>Bytell2</t>
+          <t>Angle_Droit</t>
         </is>
       </c>
       <c r="J8" s="186" t="n">
@@ -4082,7 +4082,7 @@
       </c>
       <c r="L8" s="184" t="inlineStr">
         <is>
-          <t>JLTootmy</t>
+          <t>JLKada</t>
         </is>
       </c>
       <c r="M8" s="188" t="n">
@@ -4095,7 +4095,7 @@
       </c>
       <c r="O8" s="184" t="inlineStr">
         <is>
-          <t>Hiro_Ammar</t>
+          <t>nisqylegoat</t>
         </is>
       </c>
       <c r="P8" s="184" t="n">
@@ -4125,7 +4125,7 @@
       </c>
       <c r="F9" s="177" t="inlineStr">
         <is>
-          <t>Onutrem</t>
+          <t>Etoiles</t>
         </is>
       </c>
       <c r="G9" s="177" t="n">
@@ -4151,7 +4151,7 @@
       </c>
       <c r="L9" s="177" t="inlineStr">
         <is>
-          <t>JLKada</t>
+          <t>Pepito_kawazakii</t>
         </is>
       </c>
       <c r="M9" s="192" t="n">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="F10" s="184" t="inlineStr">
         <is>
-          <t>_Linca</t>
+          <t>Onutrem</t>
         </is>
       </c>
       <c r="G10" s="184" t="n">
@@ -4198,7 +4198,7 @@
       </c>
       <c r="I10" s="184" t="inlineStr">
         <is>
-          <t>Kaatsup</t>
+          <t>KennyStream</t>
         </is>
       </c>
       <c r="J10" s="186" t="n">
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L10" s="184" t="inlineStr">
         <is>
-          <t>Wingobear</t>
+          <t>XoTrixy</t>
         </is>
       </c>
       <c r="M10" s="188" t="n">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="I11" s="177" t="inlineStr">
         <is>
-          <t>KennyStream</t>
+          <t>Kaatsup</t>
         </is>
       </c>
       <c r="J11" s="190" t="n">
@@ -4270,7 +4270,7 @@
       </c>
       <c r="L11" s="177" t="inlineStr">
         <is>
-          <t>ZeratoR</t>
+          <t>JLTootmy</t>
         </is>
       </c>
       <c r="M11" s="192" t="n">
@@ -4329,7 +4329,7 @@
       </c>
       <c r="L12" s="184" t="inlineStr">
         <is>
-          <t>Pepito_kawazakii</t>
+          <t>Maxouzboub</t>
         </is>
       </c>
       <c r="M12" s="188" t="n">
@@ -4349,7 +4349,7 @@
       </c>
       <c r="C13" s="177" t="inlineStr">
         <is>
-          <t>AntoineDaniel_</t>
+          <t>ChloeRamdani</t>
         </is>
       </c>
       <c r="D13" s="190" t="n">
@@ -4375,7 +4375,7 @@
       </c>
       <c r="I13" s="177" t="inlineStr">
         <is>
-          <t>Terraciid</t>
+          <t>ARELIANN</t>
         </is>
       </c>
       <c r="J13" s="190" t="n">
@@ -4388,7 +4388,7 @@
       </c>
       <c r="L13" s="194" t="inlineStr">
         <is>
-          <t>CrocodyleTV</t>
+          <t>Grimkujow</t>
         </is>
       </c>
       <c r="M13" s="195" t="n">
@@ -4403,7 +4403,7 @@
       <c r="A14" s="175" t="n"/>
       <c r="B14" s="196" t="inlineStr">
         <is>
-          <t>Dernière update le 05.03.25 à 01:37</t>
+          <t>Dernière update le 05.03.25 à 01:59</t>
         </is>
       </c>
       <c r="Q14" s="175" t="n"/>

</xml_diff>

<commit_message>
Top Image output feature
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1936,7 +1936,7 @@
       <c r="A14" s="101" t="n"/>
       <c r="B14" s="124" t="inlineStr">
         <is>
-          <t>Dernière update le 05.03.25 à 01:59</t>
+          <t>Dernière update le 05.03.25 à 02:46</t>
         </is>
       </c>
       <c r="Q14" s="101" t="n"/>
@@ -2753,7 +2753,7 @@
       <c r="A14" s="126" t="n"/>
       <c r="B14" s="147" t="inlineStr">
         <is>
-          <t>Dernière update le 05.03.25 à 01:59</t>
+          <t>Dernière update le 05.03.25 à 02:46</t>
         </is>
       </c>
       <c r="Q14" s="126" t="n"/>
@@ -3578,7 +3578,7 @@
       <c r="A14" s="149" t="n"/>
       <c r="B14" s="173" t="inlineStr">
         <is>
-          <t>Dernière update le 05.03.25 à 01:59</t>
+          <t>Dernière update le 05.03.25 à 02:46</t>
         </is>
       </c>
       <c r="Q14" s="149" t="n"/>
@@ -4403,7 +4403,7 @@
       <c r="A14" s="175" t="n"/>
       <c r="B14" s="196" t="inlineStr">
         <is>
-          <t>Dernière update le 05.03.25 à 01:59</t>
+          <t>Dernière update le 05.03.25 à 02:46</t>
         </is>
       </c>
       <c r="Q14" s="175" t="n"/>

</xml_diff>

<commit_message>
update and pokemon.csv fix
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1235,7 +1235,7 @@
         </is>
       </c>
       <c r="D3" s="105" t="n">
-        <v>1155</v>
+        <v>1174</v>
       </c>
       <c r="E3" s="106" t="inlineStr">
         <is>
@@ -1244,11 +1244,11 @@
       </c>
       <c r="F3" s="106" t="inlineStr">
         <is>
-          <t>NakaStream</t>
+          <t>Mickaplow</t>
         </is>
       </c>
       <c r="G3" s="106" t="n">
-        <v>815</v>
+        <v>901</v>
       </c>
       <c r="H3" s="107" t="inlineStr">
         <is>
@@ -1283,11 +1283,11 @@
       </c>
       <c r="O3" s="106" t="inlineStr">
         <is>
-          <t>Maxouzboub</t>
+          <t>Mynth0s</t>
         </is>
       </c>
       <c r="P3" s="106" t="n">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="Q3" s="101" t="n"/>
     </row>
@@ -1304,7 +1304,7 @@
         </is>
       </c>
       <c r="D4" s="113" t="n">
-        <v>1148</v>
+        <v>1172</v>
       </c>
       <c r="E4" s="114" t="inlineStr">
         <is>
@@ -1313,11 +1313,11 @@
       </c>
       <c r="F4" s="114" t="inlineStr">
         <is>
-          <t>ChloeRamdani</t>
+          <t>NakaStream</t>
         </is>
       </c>
       <c r="G4" s="114" t="n">
-        <v>807</v>
+        <v>890</v>
       </c>
       <c r="H4" s="115" t="inlineStr">
         <is>
@@ -1330,7 +1330,7 @@
         </is>
       </c>
       <c r="J4" s="116" t="n">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="K4" s="114" t="inlineStr">
         <is>
@@ -1373,7 +1373,7 @@
         </is>
       </c>
       <c r="D5" s="119" t="n">
-        <v>1112</v>
+        <v>1171</v>
       </c>
       <c r="E5" s="106" t="inlineStr">
         <is>
@@ -1382,11 +1382,11 @@
       </c>
       <c r="F5" s="106" t="inlineStr">
         <is>
-          <t>Mickaplow</t>
+          <t>Bebesukita</t>
         </is>
       </c>
       <c r="G5" s="106" t="n">
-        <v>803</v>
+        <v>850</v>
       </c>
       <c r="H5" s="120" t="inlineStr">
         <is>
@@ -1399,7 +1399,7 @@
         </is>
       </c>
       <c r="J5" s="121" t="n">
-        <v>473</v>
+        <v>510</v>
       </c>
       <c r="K5" s="106" t="inlineStr">
         <is>
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C6" s="114" t="inlineStr">
         <is>
-          <t>aypierre</t>
+          <t>JimmyBoyyy</t>
         </is>
       </c>
       <c r="D6" s="116" t="n">
-        <v>1111</v>
+        <v>1155</v>
       </c>
       <c r="E6" s="114" t="inlineStr">
         <is>
@@ -1451,11 +1451,11 @@
       </c>
       <c r="F6" s="114" t="inlineStr">
         <is>
-          <t>Brybry_</t>
+          <t>ChloeRamdani</t>
         </is>
       </c>
       <c r="G6" s="114" t="n">
-        <v>790</v>
+        <v>842</v>
       </c>
       <c r="H6" s="115" t="inlineStr">
         <is>
@@ -1507,11 +1507,11 @@
       </c>
       <c r="C7" s="106" t="inlineStr">
         <is>
-          <t>JimmyBoyyy</t>
+          <t>aypierre</t>
         </is>
       </c>
       <c r="D7" s="121" t="n">
-        <v>1100</v>
+        <v>1132</v>
       </c>
       <c r="E7" s="106" t="inlineStr">
         <is>
@@ -1546,11 +1546,11 @@
       </c>
       <c r="L7" s="106" t="inlineStr">
         <is>
-          <t>LadySundae</t>
+          <t>Maxouzboub</t>
         </is>
       </c>
       <c r="M7" s="106" t="n">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="N7" s="106" t="inlineStr">
         <is>
@@ -1580,7 +1580,7 @@
         </is>
       </c>
       <c r="D8" s="116" t="n">
-        <v>1026</v>
+        <v>1036</v>
       </c>
       <c r="E8" s="114" t="inlineStr">
         <is>
@@ -1602,11 +1602,11 @@
       </c>
       <c r="I8" s="114" t="inlineStr">
         <is>
-          <t>Grimkujow</t>
+          <t>LuttiLutti</t>
         </is>
       </c>
       <c r="J8" s="116" t="n">
-        <v>402</v>
+        <v>414</v>
       </c>
       <c r="K8" s="114" t="inlineStr">
         <is>
@@ -1615,11 +1615,11 @@
       </c>
       <c r="L8" s="114" t="inlineStr">
         <is>
-          <t>XoTrixy</t>
+          <t>LadySundae</t>
         </is>
       </c>
       <c r="M8" s="114" t="n">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="N8" s="114" t="inlineStr">
         <is>
@@ -1649,7 +1649,7 @@
         </is>
       </c>
       <c r="D9" s="121" t="n">
-        <v>985</v>
+        <v>1016</v>
       </c>
       <c r="E9" s="106" t="inlineStr">
         <is>
@@ -1658,11 +1658,11 @@
       </c>
       <c r="F9" s="106" t="inlineStr">
         <is>
-          <t>Etoiles</t>
+          <t>Theorus_</t>
         </is>
       </c>
       <c r="G9" s="106" t="n">
-        <v>659</v>
+        <v>707</v>
       </c>
       <c r="H9" s="120" t="inlineStr">
         <is>
@@ -1671,11 +1671,11 @@
       </c>
       <c r="I9" s="106" t="inlineStr">
         <is>
-          <t>LuttiLutti</t>
+          <t>Grimkujow</t>
         </is>
       </c>
       <c r="J9" s="121" t="n">
-        <v>394</v>
+        <v>402</v>
       </c>
       <c r="K9" s="106" t="inlineStr">
         <is>
@@ -1684,11 +1684,11 @@
       </c>
       <c r="L9" s="106" t="inlineStr">
         <is>
-          <t>ZeratoR</t>
+          <t>XoTrixy</t>
         </is>
       </c>
       <c r="M9" s="106" t="n">
-        <v>208</v>
+        <v>239</v>
       </c>
       <c r="N9" s="106" t="n"/>
       <c r="O9" s="106" t="n"/>
@@ -1709,7 +1709,7 @@
         </is>
       </c>
       <c r="D10" s="116" t="n">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="E10" s="114" t="inlineStr">
         <is>
@@ -1718,11 +1718,11 @@
       </c>
       <c r="F10" s="114" t="inlineStr">
         <is>
-          <t>Gom4rt_</t>
+          <t>Etoiles</t>
         </is>
       </c>
       <c r="G10" s="114" t="n">
-        <v>650</v>
+        <v>706</v>
       </c>
       <c r="H10" s="115" t="inlineStr">
         <is>
@@ -1744,11 +1744,11 @@
       </c>
       <c r="L10" s="114" t="inlineStr">
         <is>
-          <t>ARELIANN</t>
+          <t>ZeratoR</t>
         </is>
       </c>
       <c r="M10" s="114" t="n">
-        <v>179</v>
+        <v>208</v>
       </c>
       <c r="N10" s="114" t="n"/>
       <c r="O10" s="114" t="n"/>
@@ -1764,11 +1764,11 @@
       </c>
       <c r="C11" s="106" t="inlineStr">
         <is>
-          <t>Nikof_</t>
+          <t>Fukano</t>
         </is>
       </c>
       <c r="D11" s="121" t="n">
-        <v>934</v>
+        <v>960</v>
       </c>
       <c r="E11" s="106" t="inlineStr">
         <is>
@@ -1777,11 +1777,11 @@
       </c>
       <c r="F11" s="106" t="inlineStr">
         <is>
-          <t>Theorus_</t>
+          <t>Gom4rt_</t>
         </is>
       </c>
       <c r="G11" s="106" t="n">
-        <v>645</v>
+        <v>653</v>
       </c>
       <c r="H11" s="120" t="inlineStr">
         <is>
@@ -1803,11 +1803,11 @@
       </c>
       <c r="L11" s="106" t="inlineStr">
         <is>
-          <t>Hiro_Ammar</t>
+          <t>ARELIANN</t>
         </is>
       </c>
       <c r="M11" s="106" t="n">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="N11" s="106" t="n"/>
       <c r="O11" s="106" t="n"/>
@@ -1823,11 +1823,11 @@
       </c>
       <c r="C12" s="114" t="inlineStr">
         <is>
-          <t>Fukano</t>
+          <t>Nikof_</t>
         </is>
       </c>
       <c r="D12" s="116" t="n">
-        <v>916</v>
+        <v>934</v>
       </c>
       <c r="E12" s="114" t="inlineStr">
         <is>
@@ -1840,7 +1840,7 @@
         </is>
       </c>
       <c r="G12" s="114" t="n">
-        <v>638</v>
+        <v>648</v>
       </c>
       <c r="H12" s="115" t="inlineStr">
         <is>
@@ -1849,11 +1849,11 @@
       </c>
       <c r="I12" s="114" t="inlineStr">
         <is>
-          <t>Angle_Droit</t>
+          <t>KyriaaTV</t>
         </is>
       </c>
       <c r="J12" s="116" t="n">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="K12" s="114" t="inlineStr">
         <is>
@@ -1862,11 +1862,11 @@
       </c>
       <c r="L12" s="114" t="inlineStr">
         <is>
-          <t>Wingobear</t>
+          <t>Hiro_Ammar</t>
         </is>
       </c>
       <c r="M12" s="114" t="n">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="N12" s="114" t="n"/>
       <c r="O12" s="114" t="n"/>
@@ -1882,11 +1882,11 @@
       </c>
       <c r="C13" s="106" t="inlineStr">
         <is>
-          <t>Bebesukita</t>
+          <t>Brybry_</t>
         </is>
       </c>
       <c r="D13" s="121" t="n">
-        <v>850</v>
+        <v>911</v>
       </c>
       <c r="E13" s="106" t="inlineStr">
         <is>
@@ -1908,11 +1908,11 @@
       </c>
       <c r="I13" s="106" t="inlineStr">
         <is>
-          <t>KyriaaTV</t>
+          <t>Angle_Droit</t>
         </is>
       </c>
       <c r="J13" s="121" t="n">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="K13" s="123" t="inlineStr">
         <is>
@@ -1921,11 +1921,11 @@
       </c>
       <c r="L13" s="123" t="inlineStr">
         <is>
-          <t>Mynth0s</t>
+          <t>Wingobear</t>
         </is>
       </c>
       <c r="M13" s="123" t="n">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="N13" s="106" t="n"/>
       <c r="O13" s="106" t="n"/>
@@ -1936,7 +1936,7 @@
       <c r="A14" s="101" t="n"/>
       <c r="B14" s="124" t="inlineStr">
         <is>
-          <t>Dernière update le 05.03.25 à 02:46</t>
+          <t>Dernière update le 10.03.25 à 01:25</t>
         </is>
       </c>
       <c r="Q14" s="101" t="n"/>
@@ -2052,7 +2052,7 @@
         </is>
       </c>
       <c r="D3" s="105" t="n">
-        <v>633</v>
+        <v>668</v>
       </c>
       <c r="E3" s="128" t="inlineStr">
         <is>
@@ -2061,11 +2061,11 @@
       </c>
       <c r="F3" s="128" t="inlineStr">
         <is>
-          <t>_Linca</t>
+          <t>DFG_DrFeelgood</t>
         </is>
       </c>
       <c r="G3" s="128" t="n">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="H3" s="129" t="inlineStr">
         <is>
@@ -2087,7 +2087,7 @@
       </c>
       <c r="L3" s="133" t="inlineStr">
         <is>
-          <t>Onutrem</t>
+          <t>Grimkujow</t>
         </is>
       </c>
       <c r="M3" s="134" t="n">
@@ -2117,11 +2117,11 @@
       </c>
       <c r="C4" s="112" t="inlineStr">
         <is>
-          <t>GotagaTV</t>
+          <t>HexakiI</t>
         </is>
       </c>
       <c r="D4" s="113" t="n">
-        <v>573</v>
+        <v>639</v>
       </c>
       <c r="E4" s="135" t="inlineStr">
         <is>
@@ -2130,11 +2130,11 @@
       </c>
       <c r="F4" s="135" t="inlineStr">
         <is>
-          <t>Bebesukita</t>
+          <t>_Linca</t>
         </is>
       </c>
       <c r="G4" s="135" t="n">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="H4" s="136" t="inlineStr">
         <is>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="O4" s="135" t="inlineStr">
         <is>
-          <t>ZeratoR</t>
+          <t>Wingobear</t>
         </is>
       </c>
       <c r="P4" s="135" t="n">
@@ -2186,11 +2186,11 @@
       </c>
       <c r="C5" s="118" t="inlineStr">
         <is>
-          <t>HexakiI</t>
+          <t>GotagaTV</t>
         </is>
       </c>
       <c r="D5" s="119" t="n">
-        <v>506</v>
+        <v>609</v>
       </c>
       <c r="E5" s="128" t="inlineStr">
         <is>
@@ -2199,11 +2199,11 @@
       </c>
       <c r="F5" s="128" t="inlineStr">
         <is>
-          <t>JLKada</t>
+          <t>Brybry_</t>
         </is>
       </c>
       <c r="G5" s="128" t="n">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="H5" s="140" t="inlineStr">
         <is>
@@ -2216,7 +2216,7 @@
         </is>
       </c>
       <c r="J5" s="141" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="K5" s="142" t="inlineStr">
         <is>
@@ -2238,7 +2238,7 @@
       </c>
       <c r="O5" s="128" t="inlineStr">
         <is>
-          <t>Wingobear</t>
+          <t>Pepito_kawazakii</t>
         </is>
       </c>
       <c r="P5" s="128" t="n">
@@ -2268,11 +2268,11 @@
       </c>
       <c r="F6" s="135" t="inlineStr">
         <is>
-          <t>Brybry_</t>
+          <t>Bebesukita</t>
         </is>
       </c>
       <c r="G6" s="135" t="n">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="H6" s="136" t="inlineStr">
         <is>
@@ -2285,7 +2285,7 @@
         </is>
       </c>
       <c r="J6" s="137" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K6" s="138" t="inlineStr">
         <is>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="O6" s="135" t="inlineStr">
         <is>
-          <t>Pepito_kawazakii</t>
+          <t>ZeratoR</t>
         </is>
       </c>
       <c r="P6" s="135" t="n">
@@ -2328,7 +2328,7 @@
         </is>
       </c>
       <c r="D7" s="141" t="n">
-        <v>315</v>
+        <v>331</v>
       </c>
       <c r="E7" s="128" t="inlineStr">
         <is>
@@ -2337,11 +2337,11 @@
       </c>
       <c r="F7" s="128" t="inlineStr">
         <is>
-          <t>MoMaN_uS</t>
+          <t>JLKada</t>
         </is>
       </c>
       <c r="G7" s="128" t="n">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="H7" s="140" t="inlineStr">
         <is>
@@ -2397,7 +2397,7 @@
         </is>
       </c>
       <c r="D8" s="137" t="n">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="E8" s="135" t="inlineStr">
         <is>
@@ -2410,7 +2410,7 @@
         </is>
       </c>
       <c r="G8" s="135" t="n">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="H8" s="136" t="inlineStr">
         <is>
@@ -2419,11 +2419,11 @@
       </c>
       <c r="I8" s="135" t="inlineStr">
         <is>
-          <t>LuttiLutti</t>
+          <t>CrocodyleTV</t>
         </is>
       </c>
       <c r="J8" s="137" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="K8" s="138" t="inlineStr">
         <is>
@@ -2432,11 +2432,11 @@
       </c>
       <c r="L8" s="135" t="inlineStr">
         <is>
-          <t>nemenems</t>
+          <t>Maxouzboub</t>
         </is>
       </c>
       <c r="M8" s="139" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N8" s="135" t="inlineStr">
         <is>
@@ -2466,7 +2466,7 @@
         </is>
       </c>
       <c r="D9" s="141" t="n">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="E9" s="128" t="inlineStr">
         <is>
@@ -2475,11 +2475,11 @@
       </c>
       <c r="F9" s="128" t="inlineStr">
         <is>
-          <t>Mickaplow</t>
+          <t>MoMaN_uS</t>
         </is>
       </c>
       <c r="G9" s="128" t="n">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="H9" s="140" t="inlineStr">
         <is>
@@ -2488,7 +2488,7 @@
       </c>
       <c r="I9" s="128" t="inlineStr">
         <is>
-          <t>KyriaaTV</t>
+          <t>Terraciid</t>
         </is>
       </c>
       <c r="J9" s="141" t="n">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="L9" s="128" t="inlineStr">
         <is>
-          <t>Maxouzboub</t>
+          <t>nemenems</t>
         </is>
       </c>
       <c r="M9" s="143" t="n">
@@ -2522,11 +2522,11 @@
       </c>
       <c r="C10" s="135" t="inlineStr">
         <is>
-          <t>ChloeRamdani</t>
+          <t>NakaStream</t>
         </is>
       </c>
       <c r="D10" s="137" t="n">
-        <v>215</v>
+        <v>261</v>
       </c>
       <c r="E10" s="135" t="inlineStr">
         <is>
@@ -2539,7 +2539,7 @@
         </is>
       </c>
       <c r="G10" s="135" t="n">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="H10" s="136" t="inlineStr">
         <is>
@@ -2548,7 +2548,7 @@
       </c>
       <c r="I10" s="135" t="inlineStr">
         <is>
-          <t>Terraciid</t>
+          <t>KyriaaTV</t>
         </is>
       </c>
       <c r="J10" s="137" t="n">
@@ -2561,7 +2561,7 @@
       </c>
       <c r="L10" s="135" t="inlineStr">
         <is>
-          <t>Horty_</t>
+          <t>ARELIANN</t>
         </is>
       </c>
       <c r="M10" s="139" t="n">
@@ -2581,11 +2581,11 @@
       </c>
       <c r="C11" s="128" t="inlineStr">
         <is>
-          <t>NakaStream</t>
+          <t>ChloeRamdani</t>
         </is>
       </c>
       <c r="D11" s="141" t="n">
-        <v>210</v>
+        <v>229</v>
       </c>
       <c r="E11" s="128" t="inlineStr">
         <is>
@@ -2607,11 +2607,11 @@
       </c>
       <c r="I11" s="128" t="inlineStr">
         <is>
-          <t>CrocodyleTV</t>
+          <t>LuttiLutti</t>
         </is>
       </c>
       <c r="J11" s="141" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K11" s="142" t="inlineStr">
         <is>
@@ -2620,7 +2620,7 @@
       </c>
       <c r="L11" s="128" t="inlineStr">
         <is>
-          <t>ARELIANN</t>
+          <t>Horty_</t>
         </is>
       </c>
       <c r="M11" s="143" t="n">
@@ -2640,11 +2640,11 @@
       </c>
       <c r="C12" s="135" t="inlineStr">
         <is>
-          <t>DFG_DrFeelgood</t>
+          <t>JimmyBoyyy</t>
         </is>
       </c>
       <c r="D12" s="137" t="n">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="E12" s="135" t="inlineStr">
         <is>
@@ -2657,7 +2657,7 @@
         </is>
       </c>
       <c r="G12" s="135" t="n">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H12" s="136" t="inlineStr">
         <is>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="L12" s="135" t="inlineStr">
         <is>
-          <t>Elspawn</t>
+          <t>Mynth0s</t>
         </is>
       </c>
       <c r="M12" s="139" t="n">
@@ -2699,11 +2699,11 @@
       </c>
       <c r="C13" s="128" t="inlineStr">
         <is>
-          <t>JimmyBoyyy</t>
+          <t>Mickaplow</t>
         </is>
       </c>
       <c r="D13" s="141" t="n">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E13" s="128" t="inlineStr">
         <is>
@@ -2725,11 +2725,11 @@
       </c>
       <c r="I13" s="128" t="inlineStr">
         <is>
-          <t>Grimkujow</t>
+          <t>Onutrem</t>
         </is>
       </c>
       <c r="J13" s="141" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K13" s="144" t="inlineStr">
         <is>
@@ -2738,7 +2738,7 @@
       </c>
       <c r="L13" s="145" t="inlineStr">
         <is>
-          <t>Mynth0s</t>
+          <t>Elspawn</t>
         </is>
       </c>
       <c r="M13" s="146" t="n">
@@ -2753,7 +2753,7 @@
       <c r="A14" s="126" t="n"/>
       <c r="B14" s="147" t="inlineStr">
         <is>
-          <t>Dernière update le 05.03.25 à 02:46</t>
+          <t>Dernière update le 10.03.25 à 01:25</t>
         </is>
       </c>
       <c r="Q14" s="126" t="n"/>
@@ -2873,11 +2873,11 @@
       </c>
       <c r="C3" s="104" t="inlineStr">
         <is>
-          <t>GotagaTV</t>
+          <t>HexakiI</t>
         </is>
       </c>
       <c r="D3" s="105" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E3" s="151" t="inlineStr">
         <is>
@@ -2886,11 +2886,11 @@
       </c>
       <c r="F3" s="151" t="inlineStr">
         <is>
-          <t>NakaStream</t>
+          <t>Nikof_</t>
         </is>
       </c>
       <c r="G3" s="151" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H3" s="152" t="inlineStr">
         <is>
@@ -2899,7 +2899,7 @@
       </c>
       <c r="I3" s="153" t="inlineStr">
         <is>
-          <t>Kaatsup</t>
+          <t>JLTootmy</t>
         </is>
       </c>
       <c r="J3" s="154" t="n">
@@ -2912,11 +2912,11 @@
       </c>
       <c r="L3" s="156" t="inlineStr">
         <is>
-          <t>KyriaaTV</t>
+          <t>LadySundae</t>
         </is>
       </c>
       <c r="M3" s="157" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N3" s="151" t="inlineStr">
         <is>
@@ -2925,7 +2925,7 @@
       </c>
       <c r="O3" s="151" t="inlineStr">
         <is>
-          <t>Elspawn</t>
+          <t>BagheraJones</t>
         </is>
       </c>
       <c r="P3" s="151" t="n">
@@ -2942,11 +2942,11 @@
       </c>
       <c r="C4" s="112" t="inlineStr">
         <is>
-          <t>TheGuill84</t>
+          <t>GotagaTV</t>
         </is>
       </c>
       <c r="D4" s="113" t="n">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E4" s="158" t="inlineStr">
         <is>
@@ -2955,11 +2955,11 @@
       </c>
       <c r="F4" s="158" t="inlineStr">
         <is>
-          <t>Bebesukita</t>
+          <t>ChloeRamdani</t>
         </is>
       </c>
       <c r="G4" s="158" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H4" s="159" t="inlineStr">
         <is>
@@ -2968,11 +2968,11 @@
       </c>
       <c r="I4" s="158" t="inlineStr">
         <is>
-          <t>Brybry_</t>
+          <t>Kaatsup</t>
         </is>
       </c>
       <c r="J4" s="160" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K4" s="161" t="inlineStr">
         <is>
@@ -2981,11 +2981,11 @@
       </c>
       <c r="L4" s="158" t="inlineStr">
         <is>
-          <t>CrocodyleTV</t>
+          <t>XoTrixy</t>
         </is>
       </c>
       <c r="M4" s="162" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N4" s="158" t="inlineStr">
         <is>
@@ -2994,7 +2994,7 @@
       </c>
       <c r="O4" s="158" t="inlineStr">
         <is>
-          <t>ZeratoR</t>
+          <t>HarryLafranc</t>
         </is>
       </c>
       <c r="P4" s="158" t="n">
@@ -3011,11 +3011,11 @@
       </c>
       <c r="C5" s="164" t="inlineStr">
         <is>
-          <t>aypierre</t>
+          <t>TheGuill84</t>
         </is>
       </c>
       <c r="D5" s="165" t="n">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E5" s="151" t="inlineStr">
         <is>
@@ -3024,11 +3024,11 @@
       </c>
       <c r="F5" s="151" t="inlineStr">
         <is>
-          <t>ChloeRamdani</t>
+          <t>Bebesukita</t>
         </is>
       </c>
       <c r="G5" s="151" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H5" s="166" t="inlineStr">
         <is>
@@ -3050,7 +3050,7 @@
       </c>
       <c r="L5" s="151" t="inlineStr">
         <is>
-          <t>KennyStream</t>
+          <t>CrocodyleTV</t>
         </is>
       </c>
       <c r="M5" s="169" t="n">
@@ -3063,7 +3063,7 @@
       </c>
       <c r="O5" s="151" t="inlineStr">
         <is>
-          <t>HarryLafranc</t>
+          <t>Pepito_kawazakii</t>
         </is>
       </c>
       <c r="P5" s="151" t="n">
@@ -3080,11 +3080,11 @@
       </c>
       <c r="C6" s="158" t="inlineStr">
         <is>
-          <t>HexakiI</t>
+          <t>JimmyBoyyy</t>
         </is>
       </c>
       <c r="D6" s="160" t="n">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E6" s="158" t="inlineStr">
         <is>
@@ -3093,11 +3093,11 @@
       </c>
       <c r="F6" s="158" t="inlineStr">
         <is>
-          <t>JLKada</t>
+          <t>Etoiles</t>
         </is>
       </c>
       <c r="G6" s="158" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H6" s="159" t="inlineStr">
         <is>
@@ -3110,7 +3110,7 @@
         </is>
       </c>
       <c r="J6" s="160" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K6" s="161" t="inlineStr">
         <is>
@@ -3119,11 +3119,11 @@
       </c>
       <c r="L6" s="158" t="inlineStr">
         <is>
-          <t>ARELIANN</t>
+          <t>KennyStream</t>
         </is>
       </c>
       <c r="M6" s="162" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N6" s="158" t="inlineStr">
         <is>
@@ -3132,7 +3132,7 @@
       </c>
       <c r="O6" s="158" t="inlineStr">
         <is>
-          <t>Pepito_kawazakii</t>
+          <t>Horty_</t>
         </is>
       </c>
       <c r="P6" s="158" t="n">
@@ -3149,11 +3149,11 @@
       </c>
       <c r="C7" s="151" t="inlineStr">
         <is>
-          <t>Julgane</t>
+          <t>aypierre</t>
         </is>
       </c>
       <c r="D7" s="167" t="n">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="E7" s="151" t="inlineStr">
         <is>
@@ -3162,11 +3162,11 @@
       </c>
       <c r="F7" s="151" t="inlineStr">
         <is>
-          <t>AntoineDaniel_</t>
+          <t>Theorus_</t>
         </is>
       </c>
       <c r="G7" s="151" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H7" s="166" t="inlineStr">
         <is>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="L7" s="151" t="inlineStr">
         <is>
-          <t>Mynth0s</t>
+          <t>Onutrem</t>
         </is>
       </c>
       <c r="M7" s="169" t="n">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="O7" s="151" t="inlineStr">
         <is>
-          <t>Horty_</t>
+          <t>ZeratoR</t>
         </is>
       </c>
       <c r="P7" s="151" t="n">
@@ -3218,11 +3218,11 @@
       </c>
       <c r="C8" s="158" t="inlineStr">
         <is>
-          <t>DFG_DrFeelgood</t>
+          <t>Julgane</t>
         </is>
       </c>
       <c r="D8" s="160" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E8" s="158" t="inlineStr">
         <is>
@@ -3231,11 +3231,11 @@
       </c>
       <c r="F8" s="158" t="inlineStr">
         <is>
-          <t>Theorus_</t>
+          <t>JLKada</t>
         </is>
       </c>
       <c r="G8" s="158" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H8" s="159" t="inlineStr">
         <is>
@@ -3257,11 +3257,11 @@
       </c>
       <c r="L8" s="158" t="inlineStr">
         <is>
-          <t>Onutrem</t>
+          <t>ARELIANN</t>
         </is>
       </c>
       <c r="M8" s="162" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N8" s="158" t="inlineStr">
         <is>
@@ -3287,11 +3287,11 @@
       </c>
       <c r="C9" s="151" t="inlineStr">
         <is>
-          <t>_Linca</t>
+          <t>DFG_DrFeelgood</t>
         </is>
       </c>
       <c r="D9" s="167" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E9" s="151" t="inlineStr">
         <is>
@@ -3300,11 +3300,11 @@
       </c>
       <c r="F9" s="151" t="inlineStr">
         <is>
-          <t>Etoiles</t>
+          <t>Mickaplow</t>
         </is>
       </c>
       <c r="G9" s="151" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H9" s="166" t="inlineStr">
         <is>
@@ -3326,11 +3326,11 @@
       </c>
       <c r="L9" s="151" t="inlineStr">
         <is>
-          <t>Maxouzboub</t>
+          <t>Mynth0s</t>
         </is>
       </c>
       <c r="M9" s="169" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N9" s="151" t="n"/>
       <c r="O9" s="151" t="n"/>
@@ -3347,11 +3347,11 @@
       </c>
       <c r="C10" s="158" t="inlineStr">
         <is>
-          <t>JimmyBoyyy</t>
+          <t>_Linca</t>
         </is>
       </c>
       <c r="D10" s="160" t="n">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E10" s="158" t="inlineStr">
         <is>
@@ -3360,11 +3360,11 @@
       </c>
       <c r="F10" s="158" t="inlineStr">
         <is>
-          <t>Mickaplow</t>
+          <t>AntoineDaniel_</t>
         </is>
       </c>
       <c r="G10" s="158" t="n">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H10" s="159" t="inlineStr">
         <is>
@@ -3386,7 +3386,7 @@
       </c>
       <c r="L10" s="158" t="inlineStr">
         <is>
-          <t>Angle_Droit</t>
+          <t>LuttiLutti</t>
         </is>
       </c>
       <c r="M10" s="162" t="n">
@@ -3410,7 +3410,7 @@
         </is>
       </c>
       <c r="D11" s="167" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E11" s="151" t="inlineStr">
         <is>
@@ -3419,11 +3419,11 @@
       </c>
       <c r="F11" s="151" t="inlineStr">
         <is>
-          <t>MoMaN_uS</t>
+          <t>Brybry_</t>
         </is>
       </c>
       <c r="G11" s="151" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H11" s="166" t="inlineStr">
         <is>
@@ -3445,7 +3445,7 @@
       </c>
       <c r="L11" s="151" t="inlineStr">
         <is>
-          <t>LuttiLutti</t>
+          <t>Angle_Droit</t>
         </is>
       </c>
       <c r="M11" s="169" t="n">
@@ -3465,11 +3465,11 @@
       </c>
       <c r="C12" s="158" t="inlineStr">
         <is>
-          <t>Fukano</t>
+          <t>NakaStream</t>
         </is>
       </c>
       <c r="D12" s="160" t="n">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E12" s="158" t="inlineStr">
         <is>
@@ -3478,11 +3478,11 @@
       </c>
       <c r="F12" s="158" t="inlineStr">
         <is>
-          <t>Bytell2</t>
+          <t>MoMaN_uS</t>
         </is>
       </c>
       <c r="G12" s="158" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H12" s="159" t="inlineStr">
         <is>
@@ -3491,11 +3491,11 @@
       </c>
       <c r="I12" s="158" t="inlineStr">
         <is>
-          <t>LadySundae</t>
+          <t>KyriaaTV</t>
         </is>
       </c>
       <c r="J12" s="160" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K12" s="161" t="inlineStr">
         <is>
@@ -3504,7 +3504,7 @@
       </c>
       <c r="L12" s="158" t="inlineStr">
         <is>
-          <t>BagheraJones</t>
+          <t>Wingobear</t>
         </is>
       </c>
       <c r="M12" s="162" t="n">
@@ -3524,11 +3524,11 @@
       </c>
       <c r="C13" s="151" t="inlineStr">
         <is>
-          <t>Nikof_</t>
+          <t>Fukano</t>
         </is>
       </c>
       <c r="D13" s="167" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E13" s="151" t="inlineStr">
         <is>
@@ -3537,11 +3537,11 @@
       </c>
       <c r="F13" s="151" t="inlineStr">
         <is>
-          <t>JLTootmy</t>
+          <t>Bytell2</t>
         </is>
       </c>
       <c r="G13" s="151" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H13" s="166" t="inlineStr">
         <is>
@@ -3550,11 +3550,11 @@
       </c>
       <c r="I13" s="151" t="inlineStr">
         <is>
-          <t>XoTrixy</t>
+          <t>Maxouzboub</t>
         </is>
       </c>
       <c r="J13" s="167" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K13" s="170" t="inlineStr">
         <is>
@@ -3563,7 +3563,7 @@
       </c>
       <c r="L13" s="171" t="inlineStr">
         <is>
-          <t>Wingobear</t>
+          <t>Elspawn</t>
         </is>
       </c>
       <c r="M13" s="172" t="n">
@@ -3578,7 +3578,7 @@
       <c r="A14" s="149" t="n"/>
       <c r="B14" s="173" t="inlineStr">
         <is>
-          <t>Dernière update le 05.03.25 à 02:46</t>
+          <t>Dernière update le 10.03.25 à 01:25</t>
         </is>
       </c>
       <c r="Q14" s="149" t="n"/>
@@ -3702,7 +3702,7 @@
         </is>
       </c>
       <c r="D3" s="105" t="n">
-        <v>1062</v>
+        <v>1187</v>
       </c>
       <c r="E3" s="177" t="inlineStr">
         <is>
@@ -3724,11 +3724,11 @@
       </c>
       <c r="I3" s="179" t="inlineStr">
         <is>
-          <t>gobgg</t>
+          <t>Gom4rt_</t>
         </is>
       </c>
       <c r="J3" s="180" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K3" s="181" t="inlineStr">
         <is>
@@ -3737,11 +3737,11 @@
       </c>
       <c r="L3" s="182" t="inlineStr">
         <is>
-          <t>Terraciid</t>
+          <t>KennyStream</t>
         </is>
       </c>
       <c r="M3" s="183" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N3" s="177" t="inlineStr">
         <is>
@@ -3750,7 +3750,7 @@
       </c>
       <c r="O3" s="177" t="inlineStr">
         <is>
-          <t>Horty_</t>
+          <t>HarryLafranc</t>
         </is>
       </c>
       <c r="P3" s="177" t="n">
@@ -3771,7 +3771,7 @@
         </is>
       </c>
       <c r="D4" s="113" t="n">
-        <v>307</v>
+        <v>381</v>
       </c>
       <c r="E4" s="184" t="inlineStr">
         <is>
@@ -3793,11 +3793,11 @@
       </c>
       <c r="I4" s="184" t="inlineStr">
         <is>
-          <t>LittleBigWhale</t>
+          <t>nemenems</t>
         </is>
       </c>
       <c r="J4" s="186" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K4" s="187" t="inlineStr">
         <is>
@@ -3806,7 +3806,7 @@
       </c>
       <c r="L4" s="184" t="inlineStr">
         <is>
-          <t>Gom4rt_</t>
+          <t>Terraciid</t>
         </is>
       </c>
       <c r="M4" s="188" t="n">
@@ -3819,7 +3819,7 @@
       </c>
       <c r="O4" s="184" t="inlineStr">
         <is>
-          <t>HarryLafranc</t>
+          <t>Hiro_Ammar</t>
         </is>
       </c>
       <c r="P4" s="184" t="n">
@@ -3836,11 +3836,11 @@
       </c>
       <c r="C5" s="118" t="inlineStr">
         <is>
-          <t>Mickaplow</t>
+          <t>Brybry_</t>
         </is>
       </c>
       <c r="D5" s="119" t="n">
-        <v>204</v>
+        <v>273</v>
       </c>
       <c r="E5" s="177" t="inlineStr">
         <is>
@@ -3849,11 +3849,11 @@
       </c>
       <c r="F5" s="177" t="inlineStr">
         <is>
-          <t>JimmyBoyyy</t>
+          <t>MoMaN_uS</t>
         </is>
       </c>
       <c r="G5" s="177" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="189" t="inlineStr">
         <is>
@@ -3862,11 +3862,11 @@
       </c>
       <c r="I5" s="177" t="inlineStr">
         <is>
-          <t>NakaStream</t>
+          <t>gobgg</t>
         </is>
       </c>
       <c r="J5" s="190" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K5" s="191" t="inlineStr">
         <is>
@@ -3875,11 +3875,11 @@
       </c>
       <c r="L5" s="177" t="inlineStr">
         <is>
-          <t>Wingobear</t>
+          <t>ARELIANN</t>
         </is>
       </c>
       <c r="M5" s="192" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N5" s="177" t="inlineStr">
         <is>
@@ -3888,7 +3888,7 @@
       </c>
       <c r="O5" s="177" t="inlineStr">
         <is>
-          <t>Hiro_Ammar</t>
+          <t>Grimkujow</t>
         </is>
       </c>
       <c r="P5" s="177" t="n">
@@ -3909,7 +3909,7 @@
         </is>
       </c>
       <c r="D6" s="186" t="n">
-        <v>185</v>
+        <v>227</v>
       </c>
       <c r="E6" s="184" t="inlineStr">
         <is>
@@ -3918,11 +3918,11 @@
       </c>
       <c r="F6" s="184" t="inlineStr">
         <is>
-          <t>MoMaN_uS</t>
+          <t>NakaStream</t>
         </is>
       </c>
       <c r="G6" s="184" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H6" s="185" t="inlineStr">
         <is>
@@ -3931,11 +3931,11 @@
       </c>
       <c r="I6" s="184" t="inlineStr">
         <is>
-          <t>KyriaaTV</t>
+          <t>Kaatsup</t>
         </is>
       </c>
       <c r="J6" s="186" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K6" s="187" t="inlineStr">
         <is>
@@ -3944,7 +3944,7 @@
       </c>
       <c r="L6" s="184" t="inlineStr">
         <is>
-          <t>ZeratoR</t>
+          <t>Wingobear</t>
         </is>
       </c>
       <c r="M6" s="188" t="n">
@@ -3974,11 +3974,11 @@
       </c>
       <c r="C7" s="177" t="inlineStr">
         <is>
-          <t>Brybry_</t>
+          <t>DFG_DrFeelgood</t>
         </is>
       </c>
       <c r="D7" s="190" t="n">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="E7" s="177" t="inlineStr">
         <is>
@@ -4000,11 +4000,11 @@
       </c>
       <c r="I7" s="177" t="inlineStr">
         <is>
-          <t>Bytell2</t>
+          <t>KyriaaTV</t>
         </is>
       </c>
       <c r="J7" s="190" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K7" s="191" t="inlineStr">
         <is>
@@ -4069,11 +4069,11 @@
       </c>
       <c r="I8" s="184" t="inlineStr">
         <is>
-          <t>Angle_Droit</t>
+          <t>ChloeRamdani</t>
         </is>
       </c>
       <c r="J8" s="186" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K8" s="187" t="inlineStr">
         <is>
@@ -4082,7 +4082,7 @@
       </c>
       <c r="L8" s="184" t="inlineStr">
         <is>
-          <t>JLKada</t>
+          <t>ZeratoR</t>
         </is>
       </c>
       <c r="M8" s="188" t="n">
@@ -4112,11 +4112,11 @@
       </c>
       <c r="C9" s="177" t="inlineStr">
         <is>
-          <t>DFG_DrFeelgood</t>
+          <t>SakorRos</t>
         </is>
       </c>
       <c r="D9" s="190" t="n">
-        <v>155</v>
+        <v>87</v>
       </c>
       <c r="E9" s="177" t="inlineStr">
         <is>
@@ -4125,11 +4125,11 @@
       </c>
       <c r="F9" s="177" t="inlineStr">
         <is>
-          <t>Etoiles</t>
+          <t>LadySundae</t>
         </is>
       </c>
       <c r="G9" s="177" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" s="189" t="inlineStr">
         <is>
@@ -4138,11 +4138,11 @@
       </c>
       <c r="I9" s="177" t="inlineStr">
         <is>
-          <t>Elspawn</t>
+          <t>LittleBigWhale</t>
         </is>
       </c>
       <c r="J9" s="190" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K9" s="191" t="inlineStr">
         <is>
@@ -4172,11 +4172,11 @@
       </c>
       <c r="C10" s="184" t="inlineStr">
         <is>
-          <t>SakorRos</t>
+          <t>Mickaplow</t>
         </is>
       </c>
       <c r="D10" s="186" t="n">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="E10" s="184" t="inlineStr">
         <is>
@@ -4189,7 +4189,7 @@
         </is>
       </c>
       <c r="G10" s="184" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H10" s="185" t="inlineStr">
         <is>
@@ -4198,11 +4198,11 @@
       </c>
       <c r="I10" s="184" t="inlineStr">
         <is>
-          <t>KennyStream</t>
+          <t>Elspawn</t>
         </is>
       </c>
       <c r="J10" s="186" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K10" s="187" t="inlineStr">
         <is>
@@ -4231,11 +4231,11 @@
       </c>
       <c r="C11" s="177" t="inlineStr">
         <is>
-          <t>HexakiI</t>
+          <t>JimmyBoyyy</t>
         </is>
       </c>
       <c r="D11" s="190" t="n">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E11" s="177" t="inlineStr">
         <is>
@@ -4244,11 +4244,11 @@
       </c>
       <c r="F11" s="177" t="inlineStr">
         <is>
-          <t>LadySundae</t>
+          <t>Theorus_</t>
         </is>
       </c>
       <c r="G11" s="177" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" s="189" t="inlineStr">
         <is>
@@ -4257,11 +4257,11 @@
       </c>
       <c r="I11" s="177" t="inlineStr">
         <is>
-          <t>Kaatsup</t>
+          <t>Angle_Droit</t>
         </is>
       </c>
       <c r="J11" s="190" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K11" s="191" t="inlineStr">
         <is>
@@ -4290,11 +4290,11 @@
       </c>
       <c r="C12" s="184" t="inlineStr">
         <is>
-          <t>GotagaTV</t>
+          <t>HexakiI</t>
         </is>
       </c>
       <c r="D12" s="186" t="n">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E12" s="184" t="inlineStr">
         <is>
@@ -4307,7 +4307,7 @@
         </is>
       </c>
       <c r="G12" s="184" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H12" s="185" t="inlineStr">
         <is>
@@ -4316,11 +4316,11 @@
       </c>
       <c r="I12" s="184" t="inlineStr">
         <is>
-          <t>Theorus_</t>
+          <t>Etoiles</t>
         </is>
       </c>
       <c r="J12" s="186" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K12" s="187" t="inlineStr">
         <is>
@@ -4329,11 +4329,11 @@
       </c>
       <c r="L12" s="184" t="inlineStr">
         <is>
-          <t>Maxouzboub</t>
+          <t>Horty_</t>
         </is>
       </c>
       <c r="M12" s="188" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" s="184" t="n"/>
       <c r="O12" s="184" t="n"/>
@@ -4349,11 +4349,11 @@
       </c>
       <c r="C13" s="177" t="inlineStr">
         <is>
-          <t>ChloeRamdani</t>
+          <t>GotagaTV</t>
         </is>
       </c>
       <c r="D13" s="190" t="n">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E13" s="177" t="inlineStr">
         <is>
@@ -4362,11 +4362,11 @@
       </c>
       <c r="F13" s="177" t="inlineStr">
         <is>
-          <t>nemenems</t>
+          <t>JLKada</t>
         </is>
       </c>
       <c r="G13" s="177" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H13" s="189" t="inlineStr">
         <is>
@@ -4375,11 +4375,11 @@
       </c>
       <c r="I13" s="177" t="inlineStr">
         <is>
-          <t>ARELIANN</t>
+          <t>Bytell2</t>
         </is>
       </c>
       <c r="J13" s="190" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K13" s="193" t="inlineStr">
         <is>
@@ -4388,7 +4388,7 @@
       </c>
       <c r="L13" s="194" t="inlineStr">
         <is>
-          <t>Grimkujow</t>
+          <t>Maxouzboub</t>
         </is>
       </c>
       <c r="M13" s="195" t="n">
@@ -4403,7 +4403,7 @@
       <c r="A14" s="175" t="n"/>
       <c r="B14" s="196" t="inlineStr">
         <is>
-          <t>Dernière update le 05.03.25 à 02:46</t>
+          <t>Dernière update le 10.03.25 à 01:25</t>
         </is>
       </c>
       <c r="Q14" s="175" t="n"/>

</xml_diff>

<commit_message>
Option in config for leaderboards image
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1936,7 +1936,7 @@
       <c r="A14" s="101" t="n"/>
       <c r="B14" s="124" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 00:07</t>
+          <t>Dernière update le 13.03.25 à 01:14</t>
         </is>
       </c>
       <c r="Q14" s="101" t="n"/>
@@ -2753,7 +2753,7 @@
       <c r="A14" s="126" t="n"/>
       <c r="B14" s="147" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 00:07</t>
+          <t>Dernière update le 13.03.25 à 01:14</t>
         </is>
       </c>
       <c r="Q14" s="126" t="n"/>
@@ -3578,7 +3578,7 @@
       <c r="A14" s="149" t="n"/>
       <c r="B14" s="173" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 00:07</t>
+          <t>Dernière update le 13.03.25 à 01:14</t>
         </is>
       </c>
       <c r="Q14" s="149" t="n"/>
@@ -4403,7 +4403,7 @@
       <c r="A14" s="175" t="n"/>
       <c r="B14" s="196" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 00:07</t>
+          <t>Dernière update le 13.03.25 à 01:14</t>
         </is>
       </c>
       <c r="Q14" s="175" t="n"/>

</xml_diff>

<commit_message>
Can now use manually defined username in leaderboards image
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1936,7 +1936,7 @@
       <c r="A14" s="101" t="n"/>
       <c r="B14" s="124" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 01:14</t>
+          <t>Dernière update le 13.03.25 à 01:36</t>
         </is>
       </c>
       <c r="Q14" s="101" t="n"/>
@@ -2753,7 +2753,7 @@
       <c r="A14" s="126" t="n"/>
       <c r="B14" s="147" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 01:14</t>
+          <t>Dernière update le 13.03.25 à 01:36</t>
         </is>
       </c>
       <c r="Q14" s="126" t="n"/>
@@ -3578,7 +3578,7 @@
       <c r="A14" s="149" t="n"/>
       <c r="B14" s="173" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 01:14</t>
+          <t>Dernière update le 13.03.25 à 01:36</t>
         </is>
       </c>
       <c r="Q14" s="149" t="n"/>
@@ -4403,7 +4403,7 @@
       <c r="A14" s="175" t="n"/>
       <c r="B14" s="196" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 01:14</t>
+          <t>Dernière update le 13.03.25 à 01:36</t>
         </is>
       </c>
       <c r="Q14" s="175" t="n"/>

</xml_diff>

<commit_message>
Total of stats category
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1936,7 +1936,7 @@
       <c r="A14" s="101" t="n"/>
       <c r="B14" s="124" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 01:36</t>
+          <t>Dernière update le 13.03.25 à 01:53</t>
         </is>
       </c>
       <c r="Q14" s="101" t="n"/>
@@ -2753,7 +2753,7 @@
       <c r="A14" s="126" t="n"/>
       <c r="B14" s="147" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 01:36</t>
+          <t>Dernière update le 13.03.25 à 01:53</t>
         </is>
       </c>
       <c r="Q14" s="126" t="n"/>
@@ -3578,7 +3578,7 @@
       <c r="A14" s="149" t="n"/>
       <c r="B14" s="173" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 01:36</t>
+          <t>Dernière update le 13.03.25 à 01:53</t>
         </is>
       </c>
       <c r="Q14" s="149" t="n"/>
@@ -4403,7 +4403,7 @@
       <c r="A14" s="175" t="n"/>
       <c r="B14" s="196" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 01:36</t>
+          <t>Dernière update le 13.03.25 à 01:53</t>
         </is>
       </c>
       <c r="Q14" s="175" t="n"/>

</xml_diff>

<commit_message>
Leaderboard of most cobblemons of 1 type
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1936,7 +1936,7 @@
       <c r="A14" s="101" t="n"/>
       <c r="B14" s="124" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 01:53</t>
+          <t>Dernière update le 13.03.25 à 02:44</t>
         </is>
       </c>
       <c r="Q14" s="101" t="n"/>
@@ -2753,7 +2753,7 @@
       <c r="A14" s="126" t="n"/>
       <c r="B14" s="147" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 01:53</t>
+          <t>Dernière update le 13.03.25 à 02:44</t>
         </is>
       </c>
       <c r="Q14" s="126" t="n"/>
@@ -3578,7 +3578,7 @@
       <c r="A14" s="149" t="n"/>
       <c r="B14" s="173" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 01:53</t>
+          <t>Dernière update le 13.03.25 à 02:44</t>
         </is>
       </c>
       <c r="Q14" s="149" t="n"/>
@@ -4403,7 +4403,7 @@
       <c r="A14" s="175" t="n"/>
       <c r="B14" s="196" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 01:53</t>
+          <t>Dernière update le 13.03.25 à 02:44</t>
         </is>
       </c>
       <c r="Q14" s="175" t="n"/>

</xml_diff>

<commit_message>
Moved static data + added cobblemon imgs to top3
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1936,7 +1936,7 @@
       <c r="A14" s="101" t="n"/>
       <c r="B14" s="124" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 02:44</t>
+          <t>Dernière update le 13.03.25 à 11:07</t>
         </is>
       </c>
       <c r="Q14" s="101" t="n"/>
@@ -2753,7 +2753,7 @@
       <c r="A14" s="126" t="n"/>
       <c r="B14" s="147" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 02:44</t>
+          <t>Dernière update le 13.03.25 à 11:07</t>
         </is>
       </c>
       <c r="Q14" s="126" t="n"/>
@@ -3578,7 +3578,7 @@
       <c r="A14" s="149" t="n"/>
       <c r="B14" s="173" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 02:44</t>
+          <t>Dernière update le 13.03.25 à 11:07</t>
         </is>
       </c>
       <c r="Q14" s="149" t="n"/>
@@ -4403,7 +4403,7 @@
       <c r="A14" s="175" t="n"/>
       <c r="B14" s="196" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 02:44</t>
+          <t>Dernière update le 13.03.25 à 11:07</t>
         </is>
       </c>
       <c r="Q14" s="175" t="n"/>

</xml_diff>

<commit_message>
Advancements counting leaderboard for top 3
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1580,7 +1580,7 @@
         </is>
       </c>
       <c r="D8" s="116" t="n">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="E8" s="114" t="inlineStr">
         <is>
@@ -1662,7 +1662,7 @@
         </is>
       </c>
       <c r="G9" s="106" t="n">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="H9" s="120" t="inlineStr">
         <is>
@@ -1709,7 +1709,7 @@
         </is>
       </c>
       <c r="D10" s="116" t="n">
-        <v>961</v>
+        <v>964</v>
       </c>
       <c r="E10" s="114" t="inlineStr">
         <is>
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="J10" s="116" t="n">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="K10" s="114" t="inlineStr">
         <is>
@@ -1823,11 +1823,11 @@
       </c>
       <c r="C12" s="114" t="inlineStr">
         <is>
-          <t>Nikof_</t>
+          <t>Brybry_</t>
         </is>
       </c>
       <c r="D12" s="116" t="n">
-        <v>934</v>
+        <v>948</v>
       </c>
       <c r="E12" s="114" t="inlineStr">
         <is>
@@ -1853,7 +1853,7 @@
         </is>
       </c>
       <c r="J12" s="116" t="n">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="K12" s="114" t="inlineStr">
         <is>
@@ -1882,7 +1882,7 @@
       </c>
       <c r="C13" s="106" t="inlineStr">
         <is>
-          <t>Brybry_</t>
+          <t>Nikof_</t>
         </is>
       </c>
       <c r="D13" s="121" t="n">
@@ -1936,7 +1936,7 @@
       <c r="A14" s="101" t="n"/>
       <c r="B14" s="124" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 11:07</t>
+          <t>Dernière update le 13.03.25 à 17:29</t>
         </is>
       </c>
       <c r="Q14" s="101" t="n"/>
@@ -2061,11 +2061,11 @@
       </c>
       <c r="F3" s="128" t="inlineStr">
         <is>
-          <t>DFG_DrFeelgood</t>
+          <t>Mickaplow</t>
         </is>
       </c>
       <c r="G3" s="128" t="n">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="H3" s="129" t="inlineStr">
         <is>
@@ -2074,7 +2074,7 @@
       </c>
       <c r="I3" s="130" t="inlineStr">
         <is>
-          <t>AntoineDaniel_</t>
+          <t>Kaatsup</t>
         </is>
       </c>
       <c r="J3" s="131" t="n">
@@ -2087,11 +2087,11 @@
       </c>
       <c r="L3" s="133" t="inlineStr">
         <is>
-          <t>Grimkujow</t>
+          <t>JLTootmy</t>
         </is>
       </c>
       <c r="M3" s="134" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="N3" s="128" t="inlineStr">
         <is>
@@ -2130,7 +2130,7 @@
       </c>
       <c r="F4" s="135" t="inlineStr">
         <is>
-          <t>_Linca</t>
+          <t>Brybry_</t>
         </is>
       </c>
       <c r="G4" s="135" t="n">
@@ -2143,7 +2143,7 @@
       </c>
       <c r="I4" s="135" t="inlineStr">
         <is>
-          <t>Kaatsup</t>
+          <t>AntoineDaniel_</t>
         </is>
       </c>
       <c r="J4" s="137" t="n">
@@ -2156,11 +2156,11 @@
       </c>
       <c r="L4" s="135" t="inlineStr">
         <is>
-          <t>KennyStream</t>
+          <t>Grimkujow</t>
         </is>
       </c>
       <c r="M4" s="139" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N4" s="135" t="inlineStr">
         <is>
@@ -2199,11 +2199,11 @@
       </c>
       <c r="F5" s="128" t="inlineStr">
         <is>
-          <t>Brybry_</t>
+          <t>_Linca</t>
         </is>
       </c>
       <c r="G5" s="128" t="n">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H5" s="140" t="inlineStr">
         <is>
@@ -2225,11 +2225,11 @@
       </c>
       <c r="L5" s="128" t="inlineStr">
         <is>
-          <t>Angle_Droit</t>
+          <t>KennyStream</t>
         </is>
       </c>
       <c r="M5" s="143" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N5" s="128" t="inlineStr">
         <is>
@@ -2259,7 +2259,7 @@
         </is>
       </c>
       <c r="D6" s="137" t="n">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E6" s="135" t="inlineStr">
         <is>
@@ -2281,11 +2281,11 @@
       </c>
       <c r="I6" s="135" t="inlineStr">
         <is>
-          <t>LadySundae</t>
+          <t>CrocodyleTV</t>
         </is>
       </c>
       <c r="J6" s="137" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K6" s="138" t="inlineStr">
         <is>
@@ -2294,11 +2294,11 @@
       </c>
       <c r="L6" s="135" t="inlineStr">
         <is>
-          <t>XoTrixy</t>
+          <t>Angle_Droit</t>
         </is>
       </c>
       <c r="M6" s="139" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N6" s="135" t="inlineStr">
         <is>
@@ -2350,11 +2350,11 @@
       </c>
       <c r="I7" s="128" t="inlineStr">
         <is>
-          <t>CrocodyleTV</t>
+          <t>LadySundae</t>
         </is>
       </c>
       <c r="J7" s="141" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="K7" s="142" t="inlineStr">
         <is>
@@ -2363,11 +2363,11 @@
       </c>
       <c r="L7" s="128" t="inlineStr">
         <is>
-          <t>Hiro_Ammar</t>
+          <t>XoTrixy</t>
         </is>
       </c>
       <c r="M7" s="143" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="N7" s="128" t="inlineStr">
         <is>
@@ -2397,7 +2397,7 @@
         </is>
       </c>
       <c r="D8" s="137" t="n">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E8" s="135" t="inlineStr">
         <is>
@@ -2432,11 +2432,11 @@
       </c>
       <c r="L8" s="135" t="inlineStr">
         <is>
-          <t>Maxouzboub</t>
+          <t>Hiro_Ammar</t>
         </is>
       </c>
       <c r="M8" s="139" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="N8" s="135" t="inlineStr">
         <is>
@@ -2488,11 +2488,11 @@
       </c>
       <c r="I9" s="128" t="inlineStr">
         <is>
-          <t>KyriaaTV</t>
+          <t>Onutrem</t>
         </is>
       </c>
       <c r="J9" s="141" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K9" s="142" t="inlineStr">
         <is>
@@ -2501,11 +2501,11 @@
       </c>
       <c r="L9" s="128" t="inlineStr">
         <is>
-          <t>nemenems</t>
+          <t>Maxouzboub</t>
         </is>
       </c>
       <c r="M9" s="143" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N9" s="128" t="n"/>
       <c r="O9" s="128" t="n"/>
@@ -2539,7 +2539,7 @@
         </is>
       </c>
       <c r="G10" s="135" t="n">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="H10" s="136" t="inlineStr">
         <is>
@@ -2548,11 +2548,11 @@
       </c>
       <c r="I10" s="135" t="inlineStr">
         <is>
-          <t>LuttiLutti</t>
+          <t>KyriaaTV</t>
         </is>
       </c>
       <c r="J10" s="137" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K10" s="138" t="inlineStr">
         <is>
@@ -2607,11 +2607,11 @@
       </c>
       <c r="I11" s="128" t="inlineStr">
         <is>
-          <t>Terraciid</t>
+          <t>nemenems</t>
         </is>
       </c>
       <c r="J11" s="141" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K11" s="142" t="inlineStr">
         <is>
@@ -2666,11 +2666,11 @@
       </c>
       <c r="I12" s="135" t="inlineStr">
         <is>
-          <t>Onutrem</t>
+          <t>LuttiLutti</t>
         </is>
       </c>
       <c r="J12" s="137" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K12" s="138" t="inlineStr">
         <is>
@@ -2699,7 +2699,7 @@
       </c>
       <c r="C13" s="128" t="inlineStr">
         <is>
-          <t>Mickaplow</t>
+          <t>DFG_DrFeelgood</t>
         </is>
       </c>
       <c r="D13" s="141" t="n">
@@ -2725,11 +2725,11 @@
       </c>
       <c r="I13" s="128" t="inlineStr">
         <is>
-          <t>JLTootmy</t>
+          <t>Terraciid</t>
         </is>
       </c>
       <c r="J13" s="141" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="K13" s="144" t="inlineStr">
         <is>
@@ -2753,7 +2753,7 @@
       <c r="A14" s="126" t="n"/>
       <c r="B14" s="147" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 11:07</t>
+          <t>Dernière update le 13.03.25 à 17:29</t>
         </is>
       </c>
       <c r="Q14" s="126" t="n"/>
@@ -3248,7 +3248,7 @@
         </is>
       </c>
       <c r="J8" s="160" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K8" s="161" t="inlineStr">
         <is>
@@ -3291,7 +3291,7 @@
         </is>
       </c>
       <c r="D9" s="167" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E9" s="151" t="inlineStr">
         <is>
@@ -3578,7 +3578,7 @@
       <c r="A14" s="149" t="n"/>
       <c r="B14" s="173" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 11:07</t>
+          <t>Dernière update le 13.03.25 à 17:29</t>
         </is>
       </c>
       <c r="Q14" s="149" t="n"/>
@@ -3711,11 +3711,11 @@
       </c>
       <c r="F3" s="177" t="inlineStr">
         <is>
-          <t>Nikof_</t>
+          <t>TheGuill84</t>
         </is>
       </c>
       <c r="G3" s="177" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H3" s="178" t="inlineStr">
         <is>
@@ -3724,7 +3724,7 @@
       </c>
       <c r="I3" s="179" t="inlineStr">
         <is>
-          <t>ChloeRamdani</t>
+          <t>HexakiI</t>
         </is>
       </c>
       <c r="J3" s="180" t="n">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="O3" s="177" t="inlineStr">
         <is>
-          <t>HarryLafranc</t>
+          <t>CrocodyleTV</t>
         </is>
       </c>
       <c r="P3" s="177" t="n">
@@ -3780,11 +3780,11 @@
       </c>
       <c r="F4" s="184" t="inlineStr">
         <is>
-          <t>TheGuill84</t>
+          <t>MoMaN_uS</t>
         </is>
       </c>
       <c r="G4" s="184" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="185" t="inlineStr">
         <is>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="I4" s="184" t="inlineStr">
         <is>
-          <t>nemenems</t>
+          <t>ChloeRamdani</t>
         </is>
       </c>
       <c r="J4" s="186" t="n">
@@ -3819,7 +3819,7 @@
       </c>
       <c r="O4" s="184" t="inlineStr">
         <is>
-          <t>Hiro_Ammar</t>
+          <t>Maxouzboub</t>
         </is>
       </c>
       <c r="P4" s="184" t="n">
@@ -3840,7 +3840,7 @@
         </is>
       </c>
       <c r="D5" s="119" t="n">
-        <v>324</v>
+        <v>358</v>
       </c>
       <c r="E5" s="177" t="inlineStr">
         <is>
@@ -3849,7 +3849,7 @@
       </c>
       <c r="F5" s="177" t="inlineStr">
         <is>
-          <t>MoMaN_uS</t>
+          <t>_Linca</t>
         </is>
       </c>
       <c r="G5" s="177" t="n">
@@ -3862,11 +3862,11 @@
       </c>
       <c r="I5" s="177" t="inlineStr">
         <is>
-          <t>gobgg</t>
+          <t>Onutrem</t>
         </is>
       </c>
       <c r="J5" s="190" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K5" s="191" t="inlineStr">
         <is>
@@ -3888,7 +3888,7 @@
       </c>
       <c r="O5" s="177" t="inlineStr">
         <is>
-          <t>Grimkujow</t>
+          <t>HarryLafranc</t>
         </is>
       </c>
       <c r="P5" s="177" t="n">
@@ -3909,7 +3909,7 @@
         </is>
       </c>
       <c r="D6" s="186" t="n">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="E6" s="184" t="inlineStr">
         <is>
@@ -3918,11 +3918,11 @@
       </c>
       <c r="F6" s="184" t="inlineStr">
         <is>
-          <t>_Linca</t>
+          <t>LadySundae</t>
         </is>
       </c>
       <c r="G6" s="184" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H6" s="185" t="inlineStr">
         <is>
@@ -3944,7 +3944,7 @@
       </c>
       <c r="L6" s="184" t="inlineStr">
         <is>
-          <t>Mynth0s</t>
+          <t>XoTrixy</t>
         </is>
       </c>
       <c r="M6" s="188" t="n">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="O6" s="184" t="inlineStr">
         <is>
-          <t>CrocodyleTV</t>
+          <t>Grimkujow</t>
         </is>
       </c>
       <c r="P6" s="184" t="n">
@@ -3978,7 +3978,7 @@
         </is>
       </c>
       <c r="D7" s="190" t="n">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="E7" s="177" t="inlineStr">
         <is>
@@ -3987,11 +3987,11 @@
       </c>
       <c r="F7" s="177" t="inlineStr">
         <is>
-          <t>LadySundae</t>
+          <t>Theorus_</t>
         </is>
       </c>
       <c r="G7" s="177" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" s="189" t="inlineStr">
         <is>
@@ -4000,11 +4000,11 @@
       </c>
       <c r="I7" s="177" t="inlineStr">
         <is>
-          <t>Onutrem</t>
+          <t>JimmyBoyyy</t>
         </is>
       </c>
       <c r="J7" s="190" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K7" s="191" t="inlineStr">
         <is>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="L7" s="177" t="inlineStr">
         <is>
-          <t>Wingobear</t>
+          <t>Pepito_kawazakii</t>
         </is>
       </c>
       <c r="M7" s="192" t="n">
@@ -4026,7 +4026,7 @@
       </c>
       <c r="O7" s="177" t="inlineStr">
         <is>
-          <t>BagheraJones</t>
+          <t>Horty_</t>
         </is>
       </c>
       <c r="P7" s="177" t="n">
@@ -4056,11 +4056,11 @@
       </c>
       <c r="F8" s="184" t="inlineStr">
         <is>
-          <t>Theorus_</t>
+          <t>LuttiLutti</t>
         </is>
       </c>
       <c r="G8" s="184" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H8" s="185" t="inlineStr">
         <is>
@@ -4082,7 +4082,7 @@
       </c>
       <c r="L8" s="184" t="inlineStr">
         <is>
-          <t>ZeratoR</t>
+          <t>Mynth0s</t>
         </is>
       </c>
       <c r="M8" s="188" t="n">
@@ -4112,11 +4112,11 @@
       </c>
       <c r="C9" s="177" t="inlineStr">
         <is>
-          <t>SakorRos</t>
+          <t>Mickaplow</t>
         </is>
       </c>
       <c r="D9" s="190" t="n">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E9" s="177" t="inlineStr">
         <is>
@@ -4138,11 +4138,11 @@
       </c>
       <c r="I9" s="177" t="inlineStr">
         <is>
-          <t>KyriaaTV</t>
+          <t>Etoiles</t>
         </is>
       </c>
       <c r="J9" s="190" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K9" s="191" t="inlineStr">
         <is>
@@ -4151,7 +4151,7 @@
       </c>
       <c r="L9" s="177" t="inlineStr">
         <is>
-          <t>Pepito_kawazakii</t>
+          <t>ZeratoR</t>
         </is>
       </c>
       <c r="M9" s="192" t="n">
@@ -4172,11 +4172,11 @@
       </c>
       <c r="C10" s="184" t="inlineStr">
         <is>
-          <t>Mickaplow</t>
+          <t>SakorRos</t>
         </is>
       </c>
       <c r="D10" s="186" t="n">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E10" s="184" t="inlineStr">
         <is>
@@ -4185,11 +4185,11 @@
       </c>
       <c r="F10" s="184" t="inlineStr">
         <is>
-          <t>LuttiLutti</t>
+          <t>nemenems</t>
         </is>
       </c>
       <c r="G10" s="184" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H10" s="185" t="inlineStr">
         <is>
@@ -4198,7 +4198,7 @@
       </c>
       <c r="I10" s="184" t="inlineStr">
         <is>
-          <t>Bytell2</t>
+          <t>KyriaaTV</t>
         </is>
       </c>
       <c r="J10" s="186" t="n">
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L10" s="184" t="inlineStr">
         <is>
-          <t>XoTrixy</t>
+          <t>Wingobear</t>
         </is>
       </c>
       <c r="M10" s="188" t="n">
@@ -4235,7 +4235,7 @@
         </is>
       </c>
       <c r="D11" s="190" t="n">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E11" s="177" t="inlineStr">
         <is>
@@ -4244,7 +4244,7 @@
       </c>
       <c r="F11" s="177" t="inlineStr">
         <is>
-          <t>JimmyBoyyy</t>
+          <t>Gom4rt_</t>
         </is>
       </c>
       <c r="G11" s="177" t="n">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="I11" s="177" t="inlineStr">
         <is>
-          <t>Angle_Droit</t>
+          <t>Bytell2</t>
         </is>
       </c>
       <c r="J11" s="190" t="n">
@@ -4290,11 +4290,11 @@
       </c>
       <c r="C12" s="184" t="inlineStr">
         <is>
-          <t>HexakiI</t>
+          <t>AntoineDaniel_</t>
         </is>
       </c>
       <c r="D12" s="186" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E12" s="184" t="inlineStr">
         <is>
@@ -4316,7 +4316,7 @@
       </c>
       <c r="I12" s="184" t="inlineStr">
         <is>
-          <t>Elspawn</t>
+          <t>Angle_Droit</t>
         </is>
       </c>
       <c r="J12" s="186" t="n">
@@ -4329,7 +4329,7 @@
       </c>
       <c r="L12" s="184" t="inlineStr">
         <is>
-          <t>Horty_</t>
+          <t>Hiro_Ammar</t>
         </is>
       </c>
       <c r="M12" s="188" t="n">
@@ -4349,11 +4349,11 @@
       </c>
       <c r="C13" s="177" t="inlineStr">
         <is>
-          <t>AntoineDaniel_</t>
+          <t>Nikof_</t>
         </is>
       </c>
       <c r="D13" s="190" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E13" s="177" t="inlineStr">
         <is>
@@ -4362,11 +4362,11 @@
       </c>
       <c r="F13" s="177" t="inlineStr">
         <is>
-          <t>Gom4rt_</t>
+          <t>gobgg</t>
         </is>
       </c>
       <c r="G13" s="177" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H13" s="189" t="inlineStr">
         <is>
@@ -4375,11 +4375,11 @@
       </c>
       <c r="I13" s="177" t="inlineStr">
         <is>
-          <t>Etoiles</t>
+          <t>Elspawn</t>
         </is>
       </c>
       <c r="J13" s="190" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K13" s="193" t="inlineStr">
         <is>
@@ -4388,7 +4388,7 @@
       </c>
       <c r="L13" s="194" t="inlineStr">
         <is>
-          <t>Maxouzboub</t>
+          <t>BagheraJones</t>
         </is>
       </c>
       <c r="M13" s="195" t="n">
@@ -4403,7 +4403,7 @@
       <c r="A14" s="175" t="n"/>
       <c r="B14" s="196" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 11:07</t>
+          <t>Dernière update le 13.03.25 à 17:29</t>
         </is>
       </c>
       <c r="Q14" s="175" t="n"/>

</xml_diff>

<commit_message>
Waystones activated leaderboard top 3
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1936,7 +1936,7 @@
       <c r="A14" s="101" t="n"/>
       <c r="B14" s="124" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 17:29</t>
+          <t>Dernière update le 13.03.25 à 22:56</t>
         </is>
       </c>
       <c r="Q14" s="101" t="n"/>
@@ -2753,7 +2753,7 @@
       <c r="A14" s="126" t="n"/>
       <c r="B14" s="147" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 17:29</t>
+          <t>Dernière update le 13.03.25 à 22:56</t>
         </is>
       </c>
       <c r="Q14" s="126" t="n"/>
@@ -3578,7 +3578,7 @@
       <c r="A14" s="149" t="n"/>
       <c r="B14" s="173" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 17:29</t>
+          <t>Dernière update le 13.03.25 à 22:56</t>
         </is>
       </c>
       <c r="Q14" s="149" t="n"/>
@@ -4403,7 +4403,7 @@
       <c r="A14" s="175" t="n"/>
       <c r="B14" s="196" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 17:29</t>
+          <t>Dernière update le 13.03.25 à 22:56</t>
         </is>
       </c>
       <c r="Q14" s="175" t="n"/>

</xml_diff>

<commit_message>
Translate cobblemon names in fr
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1936,7 +1936,7 @@
       <c r="A14" s="101" t="n"/>
       <c r="B14" s="124" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 22:56</t>
+          <t>Dernière update le 14.03.25 à 13:09</t>
         </is>
       </c>
       <c r="Q14" s="101" t="n"/>
@@ -2753,7 +2753,7 @@
       <c r="A14" s="126" t="n"/>
       <c r="B14" s="147" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 22:56</t>
+          <t>Dernière update le 14.03.25 à 13:09</t>
         </is>
       </c>
       <c r="Q14" s="126" t="n"/>
@@ -3578,7 +3578,7 @@
       <c r="A14" s="149" t="n"/>
       <c r="B14" s="173" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 22:56</t>
+          <t>Dernière update le 14.03.25 à 13:09</t>
         </is>
       </c>
       <c r="Q14" s="149" t="n"/>
@@ -4403,7 +4403,7 @@
       <c r="A14" s="175" t="n"/>
       <c r="B14" s="196" t="inlineStr">
         <is>
-          <t>Dernière update le 13.03.25 à 22:56</t>
+          <t>Dernière update le 14.03.25 à 13:09</t>
         </is>
       </c>
       <c r="Q14" s="175" t="n"/>

</xml_diff>

<commit_message>
pvp duels network feature
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1936,7 +1936,7 @@
       <c r="A14" s="101" t="n"/>
       <c r="B14" s="124" t="inlineStr">
         <is>
-          <t>Dernière update le 14.03.25 à 16:14</t>
+          <t>Dernière update le 14.03.25 à 23:07</t>
         </is>
       </c>
       <c r="Q14" s="101" t="n"/>
@@ -2753,7 +2753,7 @@
       <c r="A14" s="126" t="n"/>
       <c r="B14" s="147" t="inlineStr">
         <is>
-          <t>Dernière update le 14.03.25 à 16:14</t>
+          <t>Dernière update le 14.03.25 à 23:07</t>
         </is>
       </c>
       <c r="Q14" s="126" t="n"/>
@@ -3578,7 +3578,7 @@
       <c r="A14" s="149" t="n"/>
       <c r="B14" s="173" t="inlineStr">
         <is>
-          <t>Dernière update le 14.03.25 à 16:14</t>
+          <t>Dernière update le 14.03.25 à 23:07</t>
         </is>
       </c>
       <c r="Q14" s="149" t="n"/>
@@ -4403,7 +4403,7 @@
       <c r="A14" s="175" t="n"/>
       <c r="B14" s="196" t="inlineStr">
         <is>
-          <t>Dernière update le 14.03.25 à 16:14</t>
+          <t>Dernière update le 14.03.25 à 23:07</t>
         </is>
       </c>
       <c r="Q14" s="175" t="n"/>

</xml_diff>

<commit_message>
Types Barchart + other minor changes
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="G4" s="114" t="n">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="H4" s="115" t="inlineStr">
         <is>
@@ -1580,7 +1580,7 @@
         </is>
       </c>
       <c r="D8" s="116" t="n">
-        <v>1064</v>
+        <v>1077</v>
       </c>
       <c r="E8" s="114" t="inlineStr">
         <is>
@@ -1619,7 +1619,7 @@
         </is>
       </c>
       <c r="M8" s="114" t="n">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="N8" s="114" t="inlineStr">
         <is>
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="J10" s="116" t="n">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="K10" s="114" t="inlineStr">
         <is>
@@ -1781,7 +1781,7 @@
         </is>
       </c>
       <c r="G11" s="106" t="n">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="H11" s="120" t="inlineStr">
         <is>
@@ -1853,7 +1853,7 @@
         </is>
       </c>
       <c r="J12" s="116" t="n">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="K12" s="114" t="inlineStr">
         <is>
@@ -1936,7 +1936,7 @@
       <c r="A14" s="101" t="n"/>
       <c r="B14" s="124" t="inlineStr">
         <is>
-          <t>Dernière update le 14.03.25 à 23:07</t>
+          <t>Dernière update le 17.03.25 à 19:11</t>
         </is>
       </c>
       <c r="Q14" s="101" t="n"/>
@@ -2048,11 +2048,11 @@
       </c>
       <c r="C3" s="104" t="inlineStr">
         <is>
-          <t>HexakiI</t>
+          <t>TheGuill84</t>
         </is>
       </c>
       <c r="D3" s="105" t="n">
-        <v>730</v>
+        <v>738</v>
       </c>
       <c r="E3" s="128" t="inlineStr">
         <is>
@@ -2074,11 +2074,11 @@
       </c>
       <c r="I3" s="130" t="inlineStr">
         <is>
-          <t>Kaatsup</t>
+          <t>nemenems</t>
         </is>
       </c>
       <c r="J3" s="131" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K3" s="132" t="inlineStr">
         <is>
@@ -2117,11 +2117,11 @@
       </c>
       <c r="C4" s="112" t="inlineStr">
         <is>
-          <t>TheGuill84</t>
+          <t>HexakiI</t>
         </is>
       </c>
       <c r="D4" s="113" t="n">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="E4" s="135" t="inlineStr">
         <is>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="I4" s="135" t="inlineStr">
         <is>
-          <t>AntoineDaniel_</t>
+          <t>Kaatsup</t>
         </is>
       </c>
       <c r="J4" s="137" t="n">
@@ -2212,11 +2212,11 @@
       </c>
       <c r="I5" s="128" t="inlineStr">
         <is>
-          <t>LittleBigWhale</t>
+          <t>AntoineDaniel_</t>
         </is>
       </c>
       <c r="J5" s="141" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K5" s="142" t="inlineStr">
         <is>
@@ -2259,7 +2259,7 @@
         </is>
       </c>
       <c r="D6" s="137" t="n">
-        <v>337</v>
+        <v>435</v>
       </c>
       <c r="E6" s="135" t="inlineStr">
         <is>
@@ -2281,11 +2281,11 @@
       </c>
       <c r="I6" s="135" t="inlineStr">
         <is>
-          <t>CrocodyleTV</t>
+          <t>LittleBigWhale</t>
         </is>
       </c>
       <c r="J6" s="137" t="n">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="K6" s="138" t="inlineStr">
         <is>
@@ -2350,11 +2350,11 @@
       </c>
       <c r="I7" s="128" t="inlineStr">
         <is>
-          <t>LadySundae</t>
+          <t>CrocodyleTV</t>
         </is>
       </c>
       <c r="J7" s="141" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K7" s="142" t="inlineStr">
         <is>
@@ -2419,11 +2419,11 @@
       </c>
       <c r="I8" s="135" t="inlineStr">
         <is>
-          <t>Bytell2</t>
+          <t>LadySundae</t>
         </is>
       </c>
       <c r="J8" s="137" t="n">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="K8" s="138" t="inlineStr">
         <is>
@@ -2488,11 +2488,11 @@
       </c>
       <c r="I9" s="128" t="inlineStr">
         <is>
-          <t>Onutrem</t>
+          <t>Bytell2</t>
         </is>
       </c>
       <c r="J9" s="141" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="K9" s="142" t="inlineStr">
         <is>
@@ -2526,7 +2526,7 @@
         </is>
       </c>
       <c r="D10" s="137" t="n">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="E10" s="135" t="inlineStr">
         <is>
@@ -2548,11 +2548,11 @@
       </c>
       <c r="I10" s="135" t="inlineStr">
         <is>
-          <t>KyriaaTV</t>
+          <t>Onutrem</t>
         </is>
       </c>
       <c r="J10" s="137" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K10" s="138" t="inlineStr">
         <is>
@@ -2607,7 +2607,7 @@
       </c>
       <c r="I11" s="128" t="inlineStr">
         <is>
-          <t>nemenems</t>
+          <t>KyriaaTV</t>
         </is>
       </c>
       <c r="J11" s="141" t="n">
@@ -2753,7 +2753,7 @@
       <c r="A14" s="126" t="n"/>
       <c r="B14" s="147" t="inlineStr">
         <is>
-          <t>Dernière update le 14.03.25 à 23:07</t>
+          <t>Dernière update le 17.03.25 à 19:11</t>
         </is>
       </c>
       <c r="Q14" s="126" t="n"/>
@@ -3175,11 +3175,11 @@
       </c>
       <c r="I7" s="151" t="inlineStr">
         <is>
-          <t>Grimkujow</t>
+          <t>nemenems</t>
         </is>
       </c>
       <c r="J7" s="167" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K7" s="168" t="inlineStr">
         <is>
@@ -3222,7 +3222,7 @@
         </is>
       </c>
       <c r="D8" s="160" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E8" s="158" t="inlineStr">
         <is>
@@ -3244,7 +3244,7 @@
       </c>
       <c r="I8" s="158" t="inlineStr">
         <is>
-          <t>nemenems</t>
+          <t>Grimkujow</t>
         </is>
       </c>
       <c r="J8" s="160" t="n">
@@ -3578,7 +3578,7 @@
       <c r="A14" s="149" t="n"/>
       <c r="B14" s="173" t="inlineStr">
         <is>
-          <t>Dernière update le 14.03.25 à 23:07</t>
+          <t>Dernière update le 17.03.25 à 19:11</t>
         </is>
       </c>
       <c r="Q14" s="149" t="n"/>
@@ -3698,11 +3698,11 @@
       </c>
       <c r="C3" s="104" t="inlineStr">
         <is>
-          <t>aypierre</t>
+          <t>NakaStream</t>
         </is>
       </c>
       <c r="D3" s="105" t="n">
-        <v>1187</v>
+        <v>6396</v>
       </c>
       <c r="E3" s="177" t="inlineStr">
         <is>
@@ -3711,11 +3711,11 @@
       </c>
       <c r="F3" s="177" t="inlineStr">
         <is>
-          <t>TheGuill84</t>
+          <t>GotagaTV</t>
         </is>
       </c>
       <c r="G3" s="177" t="n">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="H3" s="178" t="inlineStr">
         <is>
@@ -3724,7 +3724,7 @@
       </c>
       <c r="I3" s="179" t="inlineStr">
         <is>
-          <t>HexakiI</t>
+          <t>gobgg</t>
         </is>
       </c>
       <c r="J3" s="180" t="n">
@@ -3737,11 +3737,11 @@
       </c>
       <c r="L3" s="182" t="inlineStr">
         <is>
-          <t>KennyStream</t>
+          <t>ARELIANN</t>
         </is>
       </c>
       <c r="M3" s="183" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N3" s="177" t="inlineStr">
         <is>
@@ -3750,7 +3750,7 @@
       </c>
       <c r="O3" s="177" t="inlineStr">
         <is>
-          <t>CrocodyleTV</t>
+          <t>Hiro_Ammar</t>
         </is>
       </c>
       <c r="P3" s="177" t="n">
@@ -3767,11 +3767,11 @@
       </c>
       <c r="C4" s="112" t="inlineStr">
         <is>
-          <t>Fukano</t>
+          <t>Etoiles</t>
         </is>
       </c>
       <c r="D4" s="113" t="n">
-        <v>381</v>
+        <v>2484</v>
       </c>
       <c r="E4" s="184" t="inlineStr">
         <is>
@@ -3780,11 +3780,11 @@
       </c>
       <c r="F4" s="184" t="inlineStr">
         <is>
-          <t>MoMaN_uS</t>
+          <t>AntoineDaniel_</t>
         </is>
       </c>
       <c r="G4" s="184" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="H4" s="185" t="inlineStr">
         <is>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="I4" s="184" t="inlineStr">
         <is>
-          <t>ChloeRamdani</t>
+          <t>Julgane</t>
         </is>
       </c>
       <c r="J4" s="186" t="n">
@@ -3806,7 +3806,7 @@
       </c>
       <c r="L4" s="184" t="inlineStr">
         <is>
-          <t>ARELIANN</t>
+          <t>Terraciid</t>
         </is>
       </c>
       <c r="M4" s="188" t="n">
@@ -3836,11 +3836,11 @@
       </c>
       <c r="C5" s="118" t="inlineStr">
         <is>
-          <t>Brybry_</t>
+          <t>aypierre</t>
         </is>
       </c>
       <c r="D5" s="119" t="n">
-        <v>358</v>
+        <v>1187</v>
       </c>
       <c r="E5" s="177" t="inlineStr">
         <is>
@@ -3849,11 +3849,11 @@
       </c>
       <c r="F5" s="177" t="inlineStr">
         <is>
-          <t>_Linca</t>
+          <t>Nikof_</t>
         </is>
       </c>
       <c r="G5" s="177" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H5" s="189" t="inlineStr">
         <is>
@@ -3862,11 +3862,11 @@
       </c>
       <c r="I5" s="177" t="inlineStr">
         <is>
-          <t>Onutrem</t>
+          <t>HexakiI</t>
         </is>
       </c>
       <c r="J5" s="190" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K5" s="191" t="inlineStr">
         <is>
@@ -3875,11 +3875,11 @@
       </c>
       <c r="L5" s="177" t="inlineStr">
         <is>
-          <t>Terraciid</t>
+          <t>Pepito_kawazakii</t>
         </is>
       </c>
       <c r="M5" s="192" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N5" s="177" t="inlineStr">
         <is>
@@ -3888,7 +3888,7 @@
       </c>
       <c r="O5" s="177" t="inlineStr">
         <is>
-          <t>HarryLafranc</t>
+          <t>Horty_</t>
         </is>
       </c>
       <c r="P5" s="177" t="n">
@@ -3905,11 +3905,11 @@
       </c>
       <c r="C6" s="184" t="inlineStr">
         <is>
-          <t>Julgane</t>
+          <t>KyriaaTV</t>
         </is>
       </c>
       <c r="D6" s="186" t="n">
-        <v>269</v>
+        <v>697</v>
       </c>
       <c r="E6" s="184" t="inlineStr">
         <is>
@@ -3918,11 +3918,11 @@
       </c>
       <c r="F6" s="184" t="inlineStr">
         <is>
-          <t>LadySundae</t>
+          <t>_Linca</t>
         </is>
       </c>
       <c r="G6" s="184" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H6" s="185" t="inlineStr">
         <is>
@@ -3944,7 +3944,7 @@
       </c>
       <c r="L6" s="184" t="inlineStr">
         <is>
-          <t>XoTrixy</t>
+          <t>ZeratoR</t>
         </is>
       </c>
       <c r="M6" s="188" t="n">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="O6" s="184" t="inlineStr">
         <is>
-          <t>Grimkujow</t>
+          <t>TheGuill84</t>
         </is>
       </c>
       <c r="P6" s="184" t="n">
@@ -3974,11 +3974,11 @@
       </c>
       <c r="C7" s="177" t="inlineStr">
         <is>
-          <t>DFG_DrFeelgood</t>
+          <t>nemenems</t>
         </is>
       </c>
       <c r="D7" s="190" t="n">
-        <v>182</v>
+        <v>622</v>
       </c>
       <c r="E7" s="177" t="inlineStr">
         <is>
@@ -3987,11 +3987,11 @@
       </c>
       <c r="F7" s="177" t="inlineStr">
         <is>
-          <t>Theorus_</t>
+          <t>MoMaN_uS</t>
         </is>
       </c>
       <c r="G7" s="177" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H7" s="189" t="inlineStr">
         <is>
@@ -4000,11 +4000,11 @@
       </c>
       <c r="I7" s="177" t="inlineStr">
         <is>
-          <t>JimmyBoyyy</t>
+          <t>Onutrem</t>
         </is>
       </c>
       <c r="J7" s="190" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K7" s="191" t="inlineStr">
         <is>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="L7" s="177" t="inlineStr">
         <is>
-          <t>Pepito_kawazakii</t>
+          <t>XoTrixy</t>
         </is>
       </c>
       <c r="M7" s="192" t="n">
@@ -4026,7 +4026,7 @@
       </c>
       <c r="O7" s="177" t="inlineStr">
         <is>
-          <t>Horty_</t>
+          <t>Grimkujow</t>
         </is>
       </c>
       <c r="P7" s="177" t="n">
@@ -4043,11 +4043,11 @@
       </c>
       <c r="C8" s="184" t="inlineStr">
         <is>
-          <t>Bebesukita</t>
+          <t>Fukano</t>
         </is>
       </c>
       <c r="D8" s="186" t="n">
-        <v>157</v>
+        <v>381</v>
       </c>
       <c r="E8" s="184" t="inlineStr">
         <is>
@@ -4056,11 +4056,11 @@
       </c>
       <c r="F8" s="184" t="inlineStr">
         <is>
-          <t>LuttiLutti</t>
+          <t>ChloeRamdani</t>
         </is>
       </c>
       <c r="G8" s="184" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H8" s="185" t="inlineStr">
         <is>
@@ -4082,7 +4082,7 @@
       </c>
       <c r="L8" s="184" t="inlineStr">
         <is>
-          <t>Mynth0s</t>
+          <t>JLTootmy</t>
         </is>
       </c>
       <c r="M8" s="188" t="n">
@@ -4112,11 +4112,11 @@
       </c>
       <c r="C9" s="177" t="inlineStr">
         <is>
-          <t>Mickaplow</t>
+          <t>Brybry_</t>
         </is>
       </c>
       <c r="D9" s="190" t="n">
-        <v>85</v>
+        <v>358</v>
       </c>
       <c r="E9" s="177" t="inlineStr">
         <is>
@@ -4125,11 +4125,11 @@
       </c>
       <c r="F9" s="177" t="inlineStr">
         <is>
-          <t>NakaStream</t>
+          <t>LadySundae</t>
         </is>
       </c>
       <c r="G9" s="177" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H9" s="189" t="inlineStr">
         <is>
@@ -4138,11 +4138,11 @@
       </c>
       <c r="I9" s="177" t="inlineStr">
         <is>
-          <t>Etoiles</t>
+          <t>JimmyBoyyy</t>
         </is>
       </c>
       <c r="J9" s="190" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K9" s="191" t="inlineStr">
         <is>
@@ -4151,7 +4151,7 @@
       </c>
       <c r="L9" s="177" t="inlineStr">
         <is>
-          <t>ZeratoR</t>
+          <t>Wingobear</t>
         </is>
       </c>
       <c r="M9" s="192" t="n">
@@ -4172,11 +4172,11 @@
       </c>
       <c r="C10" s="184" t="inlineStr">
         <is>
-          <t>SakorRos</t>
+          <t>DFG_DrFeelgood</t>
         </is>
       </c>
       <c r="D10" s="186" t="n">
-        <v>76</v>
+        <v>281</v>
       </c>
       <c r="E10" s="184" t="inlineStr">
         <is>
@@ -4185,11 +4185,11 @@
       </c>
       <c r="F10" s="184" t="inlineStr">
         <is>
-          <t>nemenems</t>
+          <t>Theorus_</t>
         </is>
       </c>
       <c r="G10" s="184" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H10" s="185" t="inlineStr">
         <is>
@@ -4198,7 +4198,7 @@
       </c>
       <c r="I10" s="184" t="inlineStr">
         <is>
-          <t>KyriaaTV</t>
+          <t>Bytell2</t>
         </is>
       </c>
       <c r="J10" s="186" t="n">
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L10" s="184" t="inlineStr">
         <is>
-          <t>Wingobear</t>
+          <t>Mynth0s</t>
         </is>
       </c>
       <c r="M10" s="188" t="n">
@@ -4231,11 +4231,11 @@
       </c>
       <c r="C11" s="177" t="inlineStr">
         <is>
-          <t>GotagaTV</t>
+          <t>Bebesukita</t>
         </is>
       </c>
       <c r="D11" s="190" t="n">
-        <v>54</v>
+        <v>157</v>
       </c>
       <c r="E11" s="177" t="inlineStr">
         <is>
@@ -4248,7 +4248,7 @@
         </is>
       </c>
       <c r="G11" s="177" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H11" s="189" t="inlineStr">
         <is>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="I11" s="177" t="inlineStr">
         <is>
-          <t>Bytell2</t>
+          <t>Angle_Droit</t>
         </is>
       </c>
       <c r="J11" s="190" t="n">
@@ -4270,11 +4270,11 @@
       </c>
       <c r="L11" s="177" t="inlineStr">
         <is>
-          <t>JLTootmy</t>
+          <t>HarryLafranc</t>
         </is>
       </c>
       <c r="M11" s="192" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="177" t="n"/>
       <c r="O11" s="177" t="n"/>
@@ -4290,11 +4290,11 @@
       </c>
       <c r="C12" s="184" t="inlineStr">
         <is>
-          <t>AntoineDaniel_</t>
+          <t>Mickaplow</t>
         </is>
       </c>
       <c r="D12" s="186" t="n">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="E12" s="184" t="inlineStr">
         <is>
@@ -4303,11 +4303,11 @@
       </c>
       <c r="F12" s="184" t="inlineStr">
         <is>
-          <t>JLKada</t>
+          <t>LuttiLutti</t>
         </is>
       </c>
       <c r="G12" s="184" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H12" s="185" t="inlineStr">
         <is>
@@ -4316,7 +4316,7 @@
       </c>
       <c r="I12" s="184" t="inlineStr">
         <is>
-          <t>Angle_Droit</t>
+          <t>Elspawn</t>
         </is>
       </c>
       <c r="J12" s="186" t="n">
@@ -4329,7 +4329,7 @@
       </c>
       <c r="L12" s="184" t="inlineStr">
         <is>
-          <t>Hiro_Ammar</t>
+          <t>CrocodyleTV</t>
         </is>
       </c>
       <c r="M12" s="188" t="n">
@@ -4349,11 +4349,11 @@
       </c>
       <c r="C13" s="177" t="inlineStr">
         <is>
-          <t>Nikof_</t>
+          <t>SakorRos</t>
         </is>
       </c>
       <c r="D13" s="190" t="n">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="E13" s="177" t="inlineStr">
         <is>
@@ -4362,11 +4362,11 @@
       </c>
       <c r="F13" s="177" t="inlineStr">
         <is>
-          <t>gobgg</t>
+          <t>JLKada</t>
         </is>
       </c>
       <c r="G13" s="177" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H13" s="189" t="inlineStr">
         <is>
@@ -4375,11 +4375,11 @@
       </c>
       <c r="I13" s="177" t="inlineStr">
         <is>
-          <t>Elspawn</t>
+          <t>KennyStream</t>
         </is>
       </c>
       <c r="J13" s="190" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K13" s="193" t="inlineStr">
         <is>
@@ -4403,7 +4403,7 @@
       <c r="A14" s="175" t="n"/>
       <c r="B14" s="196" t="inlineStr">
         <is>
-          <t>Dernière update le 14.03.25 à 23:07</t>
+          <t>Dernière update le 17.03.25 à 19:11</t>
         </is>
       </c>
       <c r="Q14" s="175" t="n"/>

</xml_diff>

<commit_message>
Pokeballs used stats feature
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1304,7 +1304,7 @@
         </is>
       </c>
       <c r="D4" s="113" t="n">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="E4" s="114" t="inlineStr">
         <is>
@@ -1690,9 +1690,19 @@
       <c r="M9" s="106" t="n">
         <v>239</v>
       </c>
-      <c r="N9" s="106" t="n"/>
-      <c r="O9" s="106" t="n"/>
-      <c r="P9" s="106" t="n"/>
+      <c r="N9" s="106" t="inlineStr">
+        <is>
+          <t>51.</t>
+        </is>
+      </c>
+      <c r="O9" s="106" t="inlineStr">
+        <is>
+          <t>VelNewt</t>
+        </is>
+      </c>
+      <c r="P9" s="106" t="n">
+        <v>0</v>
+      </c>
       <c r="Q9" s="101" t="n"/>
       <c r="T9" s="122" t="n"/>
     </row>
@@ -1827,7 +1837,7 @@
         </is>
       </c>
       <c r="D12" s="116" t="n">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="E12" s="114" t="inlineStr">
         <is>
@@ -1936,7 +1946,7 @@
       <c r="A14" s="101" t="n"/>
       <c r="B14" s="124" t="inlineStr">
         <is>
-          <t>Dernière update le 17.03.25 à 19:11</t>
+          <t>Dernière update le 18.03.25 à 01:27</t>
         </is>
       </c>
       <c r="Q14" s="101" t="n"/>
@@ -2130,7 +2140,7 @@
       </c>
       <c r="F4" s="135" t="inlineStr">
         <is>
-          <t>Brybry_</t>
+          <t>_Linca</t>
         </is>
       </c>
       <c r="G4" s="135" t="n">
@@ -2199,7 +2209,7 @@
       </c>
       <c r="F5" s="128" t="inlineStr">
         <is>
-          <t>_Linca</t>
+          <t>Brybry_</t>
         </is>
       </c>
       <c r="G5" s="128" t="n">
@@ -2445,7 +2455,7 @@
       </c>
       <c r="O8" s="135" t="inlineStr">
         <is>
-          <t>nisqylegoat</t>
+          <t>VelNewt</t>
         </is>
       </c>
       <c r="P8" s="135" t="n">
@@ -2507,9 +2517,19 @@
       <c r="M9" s="143" t="n">
         <v>7</v>
       </c>
-      <c r="N9" s="128" t="n"/>
-      <c r="O9" s="128" t="n"/>
-      <c r="P9" s="128" t="n"/>
+      <c r="N9" s="128" t="inlineStr">
+        <is>
+          <t>51.</t>
+        </is>
+      </c>
+      <c r="O9" s="128" t="inlineStr">
+        <is>
+          <t>nisqylegoat</t>
+        </is>
+      </c>
+      <c r="P9" s="128" t="n">
+        <v>0</v>
+      </c>
       <c r="Q9" s="126" t="n"/>
       <c r="T9" s="122" t="n"/>
     </row>
@@ -2561,7 +2581,7 @@
       </c>
       <c r="L10" s="135" t="inlineStr">
         <is>
-          <t>ARELIANN</t>
+          <t>Horty_</t>
         </is>
       </c>
       <c r="M10" s="139" t="n">
@@ -2620,7 +2640,7 @@
       </c>
       <c r="L11" s="128" t="inlineStr">
         <is>
-          <t>Horty_</t>
+          <t>ARELIANN</t>
         </is>
       </c>
       <c r="M11" s="143" t="n">
@@ -2753,7 +2773,7 @@
       <c r="A14" s="126" t="n"/>
       <c r="B14" s="147" t="inlineStr">
         <is>
-          <t>Dernière update le 17.03.25 à 19:11</t>
+          <t>Dernière update le 18.03.25 à 01:27</t>
         </is>
       </c>
       <c r="Q14" s="126" t="n"/>
@@ -2912,7 +2932,7 @@
       </c>
       <c r="L3" s="156" t="inlineStr">
         <is>
-          <t>LadySundae</t>
+          <t>Maxouzboub</t>
         </is>
       </c>
       <c r="M3" s="157" t="n">
@@ -3132,7 +3152,7 @@
       </c>
       <c r="O6" s="158" t="inlineStr">
         <is>
-          <t>ZeratoR</t>
+          <t>VelNewt</t>
         </is>
       </c>
       <c r="P6" s="158" t="n">
@@ -3201,7 +3221,7 @@
       </c>
       <c r="O7" s="151" t="inlineStr">
         <is>
-          <t>Horty_</t>
+          <t>ZeratoR</t>
         </is>
       </c>
       <c r="P7" s="151" t="n">
@@ -3257,7 +3277,7 @@
       </c>
       <c r="L8" s="158" t="inlineStr">
         <is>
-          <t>Mynth0s</t>
+          <t>ARELIANN</t>
         </is>
       </c>
       <c r="M8" s="162" t="n">
@@ -3270,7 +3290,7 @@
       </c>
       <c r="O8" s="158" t="inlineStr">
         <is>
-          <t>nisqylegoat</t>
+          <t>Horty_</t>
         </is>
       </c>
       <c r="P8" s="158" t="n">
@@ -3326,15 +3346,25 @@
       </c>
       <c r="L9" s="151" t="inlineStr">
         <is>
-          <t>ARELIANN</t>
+          <t>Mynth0s</t>
         </is>
       </c>
       <c r="M9" s="169" t="n">
         <v>6</v>
       </c>
-      <c r="N9" s="151" t="n"/>
-      <c r="O9" s="151" t="n"/>
-      <c r="P9" s="151" t="n"/>
+      <c r="N9" s="151" t="inlineStr">
+        <is>
+          <t>51.</t>
+        </is>
+      </c>
+      <c r="O9" s="151" t="inlineStr">
+        <is>
+          <t>nisqylegoat</t>
+        </is>
+      </c>
+      <c r="P9" s="151" t="n">
+        <v>0</v>
+      </c>
       <c r="Q9" s="149" t="n"/>
       <c r="T9" s="122" t="n"/>
     </row>
@@ -3550,7 +3580,7 @@
       </c>
       <c r="I13" s="151" t="inlineStr">
         <is>
-          <t>Maxouzboub</t>
+          <t>LadySundae</t>
         </is>
       </c>
       <c r="J13" s="167" t="n">
@@ -3578,7 +3608,7 @@
       <c r="A14" s="149" t="n"/>
       <c r="B14" s="173" t="inlineStr">
         <is>
-          <t>Dernière update le 17.03.25 à 19:11</t>
+          <t>Dernière update le 18.03.25 à 01:27</t>
         </is>
       </c>
       <c r="Q14" s="149" t="n"/>
@@ -3737,7 +3767,7 @@
       </c>
       <c r="L3" s="182" t="inlineStr">
         <is>
-          <t>ARELIANN</t>
+          <t>Terraciid</t>
         </is>
       </c>
       <c r="M3" s="183" t="n">
@@ -3750,7 +3780,7 @@
       </c>
       <c r="O3" s="177" t="inlineStr">
         <is>
-          <t>Hiro_Ammar</t>
+          <t>HarryLafranc</t>
         </is>
       </c>
       <c r="P3" s="177" t="n">
@@ -3806,7 +3836,7 @@
       </c>
       <c r="L4" s="184" t="inlineStr">
         <is>
-          <t>Terraciid</t>
+          <t>ARELIANN</t>
         </is>
       </c>
       <c r="M4" s="188" t="n">
@@ -3875,7 +3905,7 @@
       </c>
       <c r="L5" s="177" t="inlineStr">
         <is>
-          <t>Pepito_kawazakii</t>
+          <t>ZeratoR</t>
         </is>
       </c>
       <c r="M5" s="192" t="n">
@@ -3888,7 +3918,7 @@
       </c>
       <c r="O5" s="177" t="inlineStr">
         <is>
-          <t>Horty_</t>
+          <t>VelNewt</t>
         </is>
       </c>
       <c r="P5" s="177" t="n">
@@ -3931,7 +3961,7 @@
       </c>
       <c r="I6" s="184" t="inlineStr">
         <is>
-          <t>Kaatsup</t>
+          <t>Onutrem</t>
         </is>
       </c>
       <c r="J6" s="186" t="n">
@@ -3944,7 +3974,7 @@
       </c>
       <c r="L6" s="184" t="inlineStr">
         <is>
-          <t>ZeratoR</t>
+          <t>XoTrixy</t>
         </is>
       </c>
       <c r="M6" s="188" t="n">
@@ -3957,7 +3987,7 @@
       </c>
       <c r="O6" s="184" t="inlineStr">
         <is>
-          <t>TheGuill84</t>
+          <t>Horty_</t>
         </is>
       </c>
       <c r="P6" s="184" t="n">
@@ -4000,7 +4030,7 @@
       </c>
       <c r="I7" s="177" t="inlineStr">
         <is>
-          <t>Onutrem</t>
+          <t>Kaatsup</t>
         </is>
       </c>
       <c r="J7" s="190" t="n">
@@ -4013,7 +4043,7 @@
       </c>
       <c r="L7" s="177" t="inlineStr">
         <is>
-          <t>XoTrixy</t>
+          <t>JLTootmy</t>
         </is>
       </c>
       <c r="M7" s="192" t="n">
@@ -4026,7 +4056,7 @@
       </c>
       <c r="O7" s="177" t="inlineStr">
         <is>
-          <t>Grimkujow</t>
+          <t>TheGuill84</t>
         </is>
       </c>
       <c r="P7" s="177" t="n">
@@ -4082,7 +4112,7 @@
       </c>
       <c r="L8" s="184" t="inlineStr">
         <is>
-          <t>JLTootmy</t>
+          <t>Pepito_kawazakii</t>
         </is>
       </c>
       <c r="M8" s="188" t="n">
@@ -4095,7 +4125,7 @@
       </c>
       <c r="O8" s="184" t="inlineStr">
         <is>
-          <t>nisqylegoat</t>
+          <t>Grimkujow</t>
         </is>
       </c>
       <c r="P8" s="184" t="n">
@@ -4151,15 +4181,25 @@
       </c>
       <c r="L9" s="177" t="inlineStr">
         <is>
-          <t>Wingobear</t>
+          <t>Mynth0s</t>
         </is>
       </c>
       <c r="M9" s="192" t="n">
         <v>1</v>
       </c>
-      <c r="N9" s="177" t="n"/>
-      <c r="O9" s="177" t="n"/>
-      <c r="P9" s="177" t="n"/>
+      <c r="N9" s="177" t="inlineStr">
+        <is>
+          <t>51.</t>
+        </is>
+      </c>
+      <c r="O9" s="177" t="inlineStr">
+        <is>
+          <t>nisqylegoat</t>
+        </is>
+      </c>
+      <c r="P9" s="177" t="n">
+        <v>0</v>
+      </c>
       <c r="Q9" s="175" t="n"/>
       <c r="T9" s="122" t="n"/>
     </row>
@@ -4198,7 +4238,7 @@
       </c>
       <c r="I10" s="184" t="inlineStr">
         <is>
-          <t>Bytell2</t>
+          <t>Elspawn</t>
         </is>
       </c>
       <c r="J10" s="186" t="n">
@@ -4211,7 +4251,7 @@
       </c>
       <c r="L10" s="184" t="inlineStr">
         <is>
-          <t>Mynth0s</t>
+          <t>Wingobear</t>
         </is>
       </c>
       <c r="M10" s="188" t="n">
@@ -4257,7 +4297,7 @@
       </c>
       <c r="I11" s="177" t="inlineStr">
         <is>
-          <t>Angle_Droit</t>
+          <t>Bytell2</t>
         </is>
       </c>
       <c r="J11" s="190" t="n">
@@ -4270,7 +4310,7 @@
       </c>
       <c r="L11" s="177" t="inlineStr">
         <is>
-          <t>HarryLafranc</t>
+          <t>CrocodyleTV</t>
         </is>
       </c>
       <c r="M11" s="192" t="n">
@@ -4316,7 +4356,7 @@
       </c>
       <c r="I12" s="184" t="inlineStr">
         <is>
-          <t>Elspawn</t>
+          <t>Angle_Droit</t>
         </is>
       </c>
       <c r="J12" s="186" t="n">
@@ -4329,7 +4369,7 @@
       </c>
       <c r="L12" s="184" t="inlineStr">
         <is>
-          <t>CrocodyleTV</t>
+          <t>BagheraJones</t>
         </is>
       </c>
       <c r="M12" s="188" t="n">
@@ -4388,7 +4428,7 @@
       </c>
       <c r="L13" s="194" t="inlineStr">
         <is>
-          <t>BagheraJones</t>
+          <t>Hiro_Ammar</t>
         </is>
       </c>
       <c r="M13" s="195" t="n">
@@ -4403,7 +4443,7 @@
       <c r="A14" s="175" t="n"/>
       <c r="B14" s="196" t="inlineStr">
         <is>
-          <t>Dernière update le 17.03.25 à 19:11</t>
+          <t>Dernière update le 18.03.25 à 01:27</t>
         </is>
       </c>
       <c r="Q14" s="175" t="n"/>

</xml_diff>

<commit_message>
Add gold cobblemon leaderboard in output.xlsx
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="leaderboard2" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="leaderboard3" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="leaderboard4" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="leaderboard5" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">Qui a attrapé le plus de Cobblemons ?</t>
   </si>
@@ -31,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Qui a attrapé le plus de Cobblemons légendaires ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qui a le plus de golds ?</t>
   </si>
 </sst>
 </file>
@@ -103,7 +107,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,19 +165,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF132600"/>
-        <bgColor rgb="FF261300"/>
+        <bgColor rgb="FF1F1F00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF274E00"/>
-        <bgColor rgb="FF3B7600"/>
+        <bgColor rgb="FF5D5D00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF3B7600"/>
-        <bgColor rgb="FF274E00"/>
+        <bgColor rgb="FF5D5D00"/>
       </patternFill>
     </fill>
     <fill>
@@ -185,7 +189,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF261300"/>
-        <bgColor rgb="FF132600"/>
+        <bgColor rgb="FF1F1F00"/>
       </patternFill>
     </fill>
     <fill>
@@ -203,7 +207,31 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF4E2700"/>
-        <bgColor rgb="FF763B00"/>
+        <bgColor rgb="FF1F1F00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9C9C00"/>
+        <bgColor rgb="FF7C7C00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1F1F00"/>
+        <bgColor rgb="FF132600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5D5D00"/>
+        <bgColor rgb="FF3B7600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7C7C00"/>
+        <bgColor rgb="FF5D5D00"/>
       </patternFill>
     </fill>
   </fills>
@@ -311,7 +339,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="89">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -585,6 +613,86 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="20" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="20" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="20" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="20" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="20" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="20" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="21" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="21" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="21" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="21" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="20" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="20" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="20" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="20" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="19" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="19" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -610,9 +718,9 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008400"/>
       <rgbColor rgb="FF00274E"/>
-      <rgbColor rgb="FF3B7600"/>
+      <rgbColor rgb="FF7C7C00"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF274E00"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
@@ -641,20 +749,20 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF9C9C00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFE8A202"/>
       <rgbColor rgb="FFC46200"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF5D5D00"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003B76"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF3B7600"/>
       <rgbColor rgb="FF132600"/>
       <rgbColor rgb="FF4E2700"/>
       <rgbColor rgb="FF7B3D00"/>
       <rgbColor rgb="FF9E4F00"/>
       <rgbColor rgb="FF004F9E"/>
-      <rgbColor rgb="FF274E00"/>
+      <rgbColor rgb="FF1F1F00"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -667,11 +775,11 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.48828125" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.64"/>
@@ -962,7 +1070,7 @@
       <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.35546875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.72"/>
@@ -1253,7 +1361,7 @@
       <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.35546875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.72"/>
@@ -1531,4 +1639,295 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Q1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="40.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="40.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="40.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="40.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="5.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="69"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+    </row>
+    <row r="2" customFormat="false" ht="83.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="69"/>
+      <c r="B2" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="69"/>
+    </row>
+    <row r="3" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="69"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="69"/>
+    </row>
+    <row r="4" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="69"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="69"/>
+    </row>
+    <row r="5" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="69"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="69"/>
+    </row>
+    <row r="6" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="69"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="69"/>
+    </row>
+    <row r="7" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="69"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="85"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="86"/>
+      <c r="N7" s="69"/>
+    </row>
+    <row r="8" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="69"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="78"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="78"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="69"/>
+    </row>
+    <row r="9" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="69"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="71"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="69"/>
+      <c r="Q9" s="23"/>
+    </row>
+    <row r="10" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="69"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="69"/>
+    </row>
+    <row r="11" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="69"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="83"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="84"/>
+      <c r="K11" s="85"/>
+      <c r="L11" s="71"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="69"/>
+    </row>
+    <row r="12" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="69"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="80"/>
+      <c r="K12" s="81"/>
+      <c r="L12" s="78"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="69"/>
+    </row>
+    <row r="13" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="69"/>
+      <c r="B13" s="87"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
+      <c r="J13" s="87"/>
+      <c r="K13" s="87"/>
+      <c r="L13" s="87"/>
+      <c r="M13" s="87"/>
+      <c r="N13" s="69"/>
+    </row>
+    <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="69"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="88"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="88"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="88"/>
+      <c r="L14" s="88"/>
+      <c r="M14" s="88"/>
+      <c r="N14" s="69"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="69"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="69"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B14:M14"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>